<commit_message>
Update watchlist monitor profile
avg_price month not in watchlist month will not active danger alarm
Update dailyreport template page break
</commit_message>
<xml_diff>
--- a/src/apps/dailytrans/reports/template.xlsx
+++ b/src/apps/dailytrans/reports/template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23256" windowHeight="12396"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23250" windowHeight="12390"/>
   </bookViews>
   <sheets>
     <sheet name="a week" sheetId="2" r:id="rId1"/>
@@ -1162,6 +1162,198 @@
   </si>
   <si>
     <r>
+      <t>6.75KG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>以上規格毛豬拍賣價格及土番鴨、白肉雞、雞蛋產地價格</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>—</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>中央畜產會。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">            </t>
+    </r>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>7.550KG</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>以上肉牛產地價格</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>—</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>本會畜產試驗所恆春分所及中央畜產會。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">            </t>
+    </r>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>8.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>努比亞雜交閹公羊拍賣價格</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>—</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>彰化縣肉品拍賣市場。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">            </t>
+    </r>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>9.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>紅羽土雞產地價格</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>北區、中區價格簡單平均</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>)—</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>中華民國養雞協會。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">            </t>
+    </r>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>10.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>水產品產地價格─本會漁業署。</t>
+    </r>
+    <phoneticPr fontId="20" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>5.</t>
     </r>
     <r>
@@ -1222,13 +1414,15 @@
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>枝─農產品行情報導，本會農糧署。</t>
+      <t>枝，香水百合</t>
     </r>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
     <r>
-      <t>6.75KG</t>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>5</t>
     </r>
     <r>
       <rPr>
@@ -1237,184 +1431,7 @@
         <family val="4"/>
         <charset val="136"/>
       </rPr>
-      <t>以上規格毛豬拍賣價格及土番鴨、白肉雞、雞蛋產地價格</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>—</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>中央畜產會。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">            </t>
-    </r>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>7.550KG</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>以上肉牛產地價格</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>—</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>本會畜產試驗所恆春分所及中央畜產會。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">            </t>
-    </r>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>8.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>努比亞雜交閹公羊拍賣價格</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>—</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>彰化縣肉品拍賣市場。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">            </t>
-    </r>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>9.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>紅羽土雞產地價格</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>北區、中區價格簡單平均</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>)—</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>中華民國養雞協會。</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">            </t>
-    </r>
-    <phoneticPr fontId="20" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>10.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <rFont val="標楷體"/>
-        <family val="4"/>
-        <charset val="136"/>
-      </rPr>
-      <t>水產品產地價格─本會漁業署。</t>
+      <t>枝─農產品行情報導，本會農糧署。</t>
     </r>
     <phoneticPr fontId="20" type="noConversion"/>
   </si>
@@ -2585,33 +2602,33 @@
   <dimension ref="A1:IU1893"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <pane ySplit="8" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L74" sqref="L74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="6.625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="6.625" style="6" customWidth="1"/>
     <col min="3" max="3" width="15" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" style="5" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9.109375" style="5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" style="36" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" style="24" customWidth="1"/>
-    <col min="9" max="11" width="7.88671875" style="24" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="8.77734375" style="24" customWidth="1"/>
-    <col min="13" max="19" width="8.6640625" style="27" customWidth="1"/>
-    <col min="20" max="20" width="21.44140625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="11.33203125" customWidth="1"/>
-    <col min="22" max="22" width="4.88671875" style="5" customWidth="1"/>
-    <col min="23" max="23" width="10.6640625" style="5" hidden="1" customWidth="1"/>
-    <col min="24" max="30" width="14.44140625" style="5" hidden="1" customWidth="1"/>
-    <col min="31" max="46" width="5.6640625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.375" style="5" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9.125" style="5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="10.75" style="36" customWidth="1"/>
+    <col min="8" max="8" width="10.625" style="24" customWidth="1"/>
+    <col min="9" max="11" width="7.875" style="24" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.75" style="24" customWidth="1"/>
+    <col min="13" max="19" width="8.625" style="27" customWidth="1"/>
+    <col min="20" max="20" width="21.5" style="1" customWidth="1"/>
+    <col min="21" max="21" width="11.375" customWidth="1"/>
+    <col min="22" max="22" width="4.875" style="5" customWidth="1"/>
+    <col min="23" max="23" width="10.625" style="5" hidden="1" customWidth="1"/>
+    <col min="24" max="30" width="14.5" style="5" hidden="1" customWidth="1"/>
+    <col min="31" max="46" width="5.625" style="5" customWidth="1"/>
     <col min="47" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="11.4" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:32" ht="11.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="13"/>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -2625,7 +2642,7 @@
       <c r="M1" s="26"/>
       <c r="N1" s="26"/>
     </row>
-    <row r="2" spans="1:32" s="50" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:32" s="50" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="112" t="s">
         <v>201</v>
       </c>
@@ -2650,7 +2667,7 @@
       <c r="T2" s="113"/>
       <c r="U2" s="113"/>
     </row>
-    <row r="3" spans="1:32" ht="11.4" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:32" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="77"/>
       <c r="B3" s="78"/>
       <c r="C3" s="78"/>
@@ -2673,7 +2690,7 @@
       <c r="T3" s="78"/>
       <c r="U3" s="78"/>
     </row>
-    <row r="4" spans="1:32" ht="4.95" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:32" ht="4.9000000000000004" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
       <c r="D4" s="2"/>
@@ -2688,7 +2705,7 @@
       <c r="M4" s="26"/>
       <c r="N4" s="26"/>
     </row>
-    <row r="5" spans="1:32" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
       <c r="D5" s="3"/>
@@ -2712,7 +2729,7 @@
       </c>
       <c r="U5" s="135"/>
     </row>
-    <row r="6" spans="1:32" s="4" customFormat="1" ht="31.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" s="4" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="116" t="s">
         <v>0</v>
       </c>
@@ -2754,7 +2771,7 @@
       <c r="AE6" s="50"/>
       <c r="AF6" s="50"/>
     </row>
-    <row r="7" spans="1:32" s="4" customFormat="1" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:32" s="4" customFormat="1" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="119"/>
       <c r="B7" s="120"/>
       <c r="C7" s="121"/>
@@ -2796,7 +2813,7 @@
       <c r="AE7" s="50"/>
       <c r="AF7" s="50"/>
     </row>
-    <row r="8" spans="1:32" s="4" customFormat="1" ht="48.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" s="4" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A8" s="122"/>
       <c r="B8" s="123"/>
       <c r="C8" s="124"/>
@@ -2870,7 +2887,7 @@
       <c r="AE8" s="50"/>
       <c r="AF8" s="50"/>
     </row>
-    <row r="9" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="s">
         <v>7</v>
       </c>
@@ -2955,7 +2972,7 @@
       <c r="AE9" s="50"/>
       <c r="AF9" s="50"/>
     </row>
-    <row r="10" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
         <v>9</v>
       </c>
@@ -3038,7 +3055,7 @@
       <c r="AE10" s="50"/>
       <c r="AF10" s="50"/>
     </row>
-    <row r="11" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="s">
         <v>11</v>
       </c>
@@ -3127,7 +3144,7 @@
       <c r="AE11" s="50"/>
       <c r="AF11" s="50"/>
     </row>
-    <row r="12" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="s">
         <v>13</v>
       </c>
@@ -3216,7 +3233,7 @@
       <c r="AE12" s="50"/>
       <c r="AF12" s="50"/>
     </row>
-    <row r="13" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="s">
         <v>15</v>
       </c>
@@ -3305,7 +3322,7 @@
       <c r="AE13" s="50"/>
       <c r="AF13" s="50"/>
     </row>
-    <row r="14" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
         <v>17</v>
       </c>
@@ -3391,7 +3408,7 @@
       <c r="AE14" s="50"/>
       <c r="AF14" s="50"/>
     </row>
-    <row r="15" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="s">
         <v>19</v>
       </c>
@@ -3476,7 +3493,7 @@
       <c r="AE15" s="50"/>
       <c r="AF15" s="50"/>
     </row>
-    <row r="16" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="s">
         <v>21</v>
       </c>
@@ -3561,7 +3578,7 @@
       <c r="AE16" s="50"/>
       <c r="AF16" s="50"/>
     </row>
-    <row r="17" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="s">
         <v>23</v>
       </c>
@@ -3646,7 +3663,7 @@
       <c r="AE17" s="50"/>
       <c r="AF17" s="50"/>
     </row>
-    <row r="18" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="s">
         <v>25</v>
       </c>
@@ -3731,7 +3748,7 @@
       <c r="AE18" s="50"/>
       <c r="AF18" s="50"/>
     </row>
-    <row r="19" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="s">
         <v>27</v>
       </c>
@@ -3816,7 +3833,7 @@
       <c r="AE19" s="50"/>
       <c r="AF19" s="50"/>
     </row>
-    <row r="20" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="s">
         <v>29</v>
       </c>
@@ -3901,7 +3918,7 @@
       <c r="AE20" s="50"/>
       <c r="AF20" s="50"/>
     </row>
-    <row r="21" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="s">
         <v>31</v>
       </c>
@@ -3986,7 +4003,7 @@
       <c r="AE21" s="50"/>
       <c r="AF21" s="50"/>
     </row>
-    <row r="22" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="s">
         <v>33</v>
       </c>
@@ -4071,7 +4088,7 @@
       <c r="AE22" s="50"/>
       <c r="AF22" s="50"/>
     </row>
-    <row r="23" spans="1:32" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:32" s="4" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="s">
         <v>35</v>
       </c>
@@ -4156,7 +4173,7 @@
       <c r="AE23" s="50"/>
       <c r="AF23" s="50"/>
     </row>
-    <row r="24" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="s">
         <v>36</v>
       </c>
@@ -4241,7 +4258,7 @@
       <c r="AE24" s="50"/>
       <c r="AF24" s="50"/>
     </row>
-    <row r="25" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
         <v>38</v>
       </c>
@@ -4326,7 +4343,7 @@
       <c r="AE25" s="50"/>
       <c r="AF25" s="50"/>
     </row>
-    <row r="26" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="s">
         <v>40</v>
       </c>
@@ -4411,7 +4428,7 @@
       <c r="AE26" s="50"/>
       <c r="AF26" s="50"/>
     </row>
-    <row r="27" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
         <v>42</v>
       </c>
@@ -4496,7 +4513,7 @@
       <c r="AE27" s="50"/>
       <c r="AF27" s="50"/>
     </row>
-    <row r="28" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="s">
         <v>44</v>
       </c>
@@ -4581,7 +4598,7 @@
       <c r="AE28" s="50"/>
       <c r="AF28" s="50"/>
     </row>
-    <row r="29" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="40" t="s">
         <v>46</v>
       </c>
@@ -4667,7 +4684,7 @@
       <c r="AE29" s="50"/>
       <c r="AF29" s="50"/>
     </row>
-    <row r="30" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="s">
         <v>48</v>
       </c>
@@ -4753,7 +4770,7 @@
       <c r="AE30" s="50"/>
       <c r="AF30" s="50"/>
     </row>
-    <row r="31" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="s">
         <v>50</v>
       </c>
@@ -4838,7 +4855,7 @@
       <c r="AE31" s="50"/>
       <c r="AF31" s="50"/>
     </row>
-    <row r="32" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
         <v>52</v>
       </c>
@@ -4923,7 +4940,7 @@
       <c r="AE32" s="50"/>
       <c r="AF32" s="50"/>
     </row>
-    <row r="33" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="40" t="s">
         <v>54</v>
       </c>
@@ -5009,7 +5026,7 @@
       <c r="AE33" s="50"/>
       <c r="AF33" s="50"/>
     </row>
-    <row r="34" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="s">
         <v>56</v>
       </c>
@@ -5094,7 +5111,7 @@
       <c r="AE34" s="50"/>
       <c r="AF34" s="50"/>
     </row>
-    <row r="35" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="s">
         <v>58</v>
       </c>
@@ -5179,7 +5196,7 @@
       <c r="AE35" s="50"/>
       <c r="AF35" s="50"/>
     </row>
-    <row r="36" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="s">
         <v>60</v>
       </c>
@@ -5264,7 +5281,7 @@
       <c r="AE36" s="50"/>
       <c r="AF36" s="50"/>
     </row>
-    <row r="37" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="40" t="s">
         <v>62</v>
       </c>
@@ -5349,7 +5366,7 @@
       <c r="AE37" s="50"/>
       <c r="AF37" s="50"/>
     </row>
-    <row r="38" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="s">
         <v>64</v>
       </c>
@@ -5434,7 +5451,7 @@
       <c r="AE38" s="50"/>
       <c r="AF38" s="50"/>
     </row>
-    <row r="39" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="40" t="s">
         <v>66</v>
       </c>
@@ -5519,7 +5536,7 @@
       <c r="AE39" s="50"/>
       <c r="AF39" s="50"/>
     </row>
-    <row r="40" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="40" t="s">
         <v>68</v>
       </c>
@@ -5604,7 +5621,7 @@
       <c r="AE40" s="50"/>
       <c r="AF40" s="50"/>
     </row>
-    <row r="41" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="40" t="s">
         <v>70</v>
       </c>
@@ -5689,7 +5706,7 @@
       <c r="AE41" s="50"/>
       <c r="AF41" s="50"/>
     </row>
-    <row r="42" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="40" t="s">
         <v>72</v>
       </c>
@@ -5775,7 +5792,7 @@
       <c r="AE42" s="50"/>
       <c r="AF42" s="50"/>
     </row>
-    <row r="43" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="40" t="s">
         <v>74</v>
       </c>
@@ -5860,7 +5877,7 @@
       <c r="AE43" s="50"/>
       <c r="AF43" s="50"/>
     </row>
-    <row r="44" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="40" t="s">
         <v>76</v>
       </c>
@@ -5945,7 +5962,7 @@
       <c r="AE44" s="50"/>
       <c r="AF44" s="50"/>
     </row>
-    <row r="45" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="40" t="s">
         <v>78</v>
       </c>
@@ -6030,7 +6047,7 @@
       <c r="AE45" s="50"/>
       <c r="AF45" s="50"/>
     </row>
-    <row r="46" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="40" t="s">
         <v>80</v>
       </c>
@@ -6115,7 +6132,7 @@
       <c r="AE46" s="50"/>
       <c r="AF46" s="50"/>
     </row>
-    <row r="47" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="40" t="s">
         <v>81</v>
       </c>
@@ -6200,7 +6217,7 @@
       <c r="AE47" s="50"/>
       <c r="AF47" s="50"/>
     </row>
-    <row r="48" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="40" t="s">
         <v>82</v>
       </c>
@@ -6285,7 +6302,7 @@
       <c r="AE48" s="50"/>
       <c r="AF48" s="50"/>
     </row>
-    <row r="49" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="40" t="s">
         <v>83</v>
       </c>
@@ -6370,7 +6387,7 @@
       <c r="AE49" s="50"/>
       <c r="AF49" s="50"/>
     </row>
-    <row r="50" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="40" t="s">
         <v>84</v>
       </c>
@@ -6455,7 +6472,7 @@
       <c r="AE50" s="50"/>
       <c r="AF50" s="50"/>
     </row>
-    <row r="51" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="40" t="s">
         <v>85</v>
       </c>
@@ -6540,7 +6557,7 @@
       <c r="AE51" s="50"/>
       <c r="AF51" s="50"/>
     </row>
-    <row r="52" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="40" t="s">
         <v>86</v>
       </c>
@@ -6625,7 +6642,7 @@
       <c r="AE52" s="50"/>
       <c r="AF52" s="50"/>
     </row>
-    <row r="53" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="40" t="s">
         <v>87</v>
       </c>
@@ -6710,7 +6727,7 @@
       <c r="AE53" s="50"/>
       <c r="AF53" s="50"/>
     </row>
-    <row r="54" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="40" t="s">
         <v>88</v>
       </c>
@@ -6795,7 +6812,7 @@
       <c r="AE54" s="50"/>
       <c r="AF54" s="50"/>
     </row>
-    <row r="55" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="40" t="s">
         <v>89</v>
       </c>
@@ -6880,7 +6897,7 @@
       <c r="AE55" s="50"/>
       <c r="AF55" s="50"/>
     </row>
-    <row r="56" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="40" t="s">
         <v>90</v>
       </c>
@@ -6965,7 +6982,7 @@
       <c r="AE56" s="50"/>
       <c r="AF56" s="50"/>
     </row>
-    <row r="57" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="40" t="s">
         <v>92</v>
       </c>
@@ -7050,7 +7067,7 @@
       <c r="AE57" s="50"/>
       <c r="AF57" s="50"/>
     </row>
-    <row r="58" spans="1:32" s="37" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:32" s="37" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="40" t="s">
         <v>94</v>
       </c>
@@ -7133,7 +7150,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="59" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="40" t="s">
         <v>96</v>
       </c>
@@ -7218,7 +7235,7 @@
       <c r="AE59" s="50"/>
       <c r="AF59" s="50"/>
     </row>
-    <row r="60" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="40" t="s">
         <v>98</v>
       </c>
@@ -7303,7 +7320,7 @@
       <c r="AE60" s="50"/>
       <c r="AF60" s="50"/>
     </row>
-    <row r="61" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="40" t="s">
         <v>100</v>
       </c>
@@ -7388,7 +7405,7 @@
       <c r="AE61" s="50"/>
       <c r="AF61" s="50"/>
     </row>
-    <row r="62" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="40" t="s">
         <v>102</v>
       </c>
@@ -7474,7 +7491,7 @@
       <c r="AE62" s="50"/>
       <c r="AF62" s="50"/>
     </row>
-    <row r="63" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="40" t="s">
         <v>104</v>
       </c>
@@ -7559,7 +7576,7 @@
       <c r="AE63" s="50"/>
       <c r="AF63" s="50"/>
     </row>
-    <row r="64" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="40" t="s">
         <v>106</v>
       </c>
@@ -7645,7 +7662,7 @@
       <c r="AE64" s="50"/>
       <c r="AF64" s="50"/>
     </row>
-    <row r="65" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="40" t="s">
         <v>108</v>
       </c>
@@ -7730,7 +7747,7 @@
       <c r="AE65" s="50"/>
       <c r="AF65" s="50"/>
     </row>
-    <row r="66" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="40" t="s">
         <v>110</v>
       </c>
@@ -7816,7 +7833,7 @@
       <c r="AE66" s="50"/>
       <c r="AF66" s="50"/>
     </row>
-    <row r="67" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="40" t="s">
         <v>112</v>
       </c>
@@ -7901,7 +7918,7 @@
       <c r="AE67" s="50"/>
       <c r="AF67" s="50"/>
     </row>
-    <row r="68" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="40" t="s">
         <v>114</v>
       </c>
@@ -7986,7 +8003,7 @@
       <c r="AE68" s="50"/>
       <c r="AF68" s="50"/>
     </row>
-    <row r="69" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="40" t="s">
         <v>116</v>
       </c>
@@ -8072,7 +8089,7 @@
       <c r="AE69" s="50"/>
       <c r="AF69" s="50"/>
     </row>
-    <row r="70" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="40" t="s">
         <v>118</v>
       </c>
@@ -8157,7 +8174,7 @@
       <c r="AE70" s="50"/>
       <c r="AF70" s="50"/>
     </row>
-    <row r="71" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="40" t="s">
         <v>120</v>
       </c>
@@ -8243,7 +8260,7 @@
       <c r="AE71" s="50"/>
       <c r="AF71" s="50"/>
     </row>
-    <row r="72" spans="1:32" s="50" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:32" s="50" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="72"/>
       <c r="B72" s="89" t="s">
         <v>205</v>
@@ -8325,7 +8342,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="73" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="39"/>
       <c r="B73" s="109" t="s">
         <v>202</v>
@@ -8410,7 +8427,7 @@
       <c r="AE73" s="50"/>
       <c r="AF73" s="50"/>
     </row>
-    <row r="74" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="40" t="s">
         <v>121</v>
       </c>
@@ -8495,7 +8512,7 @@
       <c r="AE74" s="50"/>
       <c r="AF74" s="50"/>
     </row>
-    <row r="75" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="40" t="s">
         <v>123</v>
       </c>
@@ -8580,7 +8597,7 @@
       <c r="AE75" s="50"/>
       <c r="AF75" s="50"/>
     </row>
-    <row r="76" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="40" t="s">
         <v>124</v>
       </c>
@@ -8666,7 +8683,7 @@
       <c r="AE76" s="50"/>
       <c r="AF76" s="50"/>
     </row>
-    <row r="77" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="40">
         <v>0</v>
       </c>
@@ -8751,7 +8768,7 @@
       <c r="AE77" s="50"/>
       <c r="AF77" s="50"/>
     </row>
-    <row r="78" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="40" t="s">
         <v>127</v>
       </c>
@@ -8837,7 +8854,7 @@
       <c r="AE78" s="50"/>
       <c r="AF78" s="50"/>
     </row>
-    <row r="79" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="40" t="s">
         <v>129</v>
       </c>
@@ -8923,7 +8940,7 @@
       <c r="AE79" s="50"/>
       <c r="AF79" s="50"/>
     </row>
-    <row r="80" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="40" t="s">
         <v>131</v>
       </c>
@@ -9008,7 +9025,7 @@
       <c r="AE80" s="50"/>
       <c r="AF80" s="50"/>
     </row>
-    <row r="81" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="40" t="s">
         <v>133</v>
       </c>
@@ -9093,7 +9110,7 @@
       <c r="AE81" s="50"/>
       <c r="AF81" s="50"/>
     </row>
-    <row r="82" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="40" t="s">
         <v>135</v>
       </c>
@@ -9179,7 +9196,7 @@
       <c r="AE82" s="50"/>
       <c r="AF82" s="50"/>
     </row>
-    <row r="83" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="40" t="s">
         <v>137</v>
       </c>
@@ -9265,7 +9282,7 @@
       <c r="AE83" s="50"/>
       <c r="AF83" s="50"/>
     </row>
-    <row r="84" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="40" t="s">
         <v>139</v>
       </c>
@@ -9351,7 +9368,7 @@
       <c r="AE84" s="50"/>
       <c r="AF84" s="50"/>
     </row>
-    <row r="85" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="40" t="s">
         <v>141</v>
       </c>
@@ -9437,7 +9454,7 @@
       <c r="AE85" s="50"/>
       <c r="AF85" s="50"/>
     </row>
-    <row r="86" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="40" t="s">
         <v>143</v>
       </c>
@@ -9523,7 +9540,7 @@
       <c r="AE86" s="50"/>
       <c r="AF86" s="50"/>
     </row>
-    <row r="87" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="40" t="s">
         <v>145</v>
       </c>
@@ -9609,7 +9626,7 @@
       <c r="AE87" s="50"/>
       <c r="AF87" s="50"/>
     </row>
-    <row r="88" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="40" t="s">
         <v>147</v>
       </c>
@@ -9694,7 +9711,7 @@
       <c r="AE88" s="50"/>
       <c r="AF88" s="50"/>
     </row>
-    <row r="89" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="40" t="s">
         <v>148</v>
       </c>
@@ -9779,7 +9796,7 @@
       <c r="AE89" s="50"/>
       <c r="AF89" s="50"/>
     </row>
-    <row r="90" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="40" t="s">
         <v>149</v>
       </c>
@@ -9864,7 +9881,7 @@
       <c r="AE90" s="50"/>
       <c r="AF90" s="50"/>
     </row>
-    <row r="91" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="40" t="s">
         <v>150</v>
       </c>
@@ -9949,7 +9966,7 @@
       <c r="AE91" s="50"/>
       <c r="AF91" s="50"/>
     </row>
-    <row r="92" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="40" t="s">
         <v>151</v>
       </c>
@@ -10034,7 +10051,7 @@
       <c r="AE92" s="50"/>
       <c r="AF92" s="50"/>
     </row>
-    <row r="93" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="40" t="s">
         <v>152</v>
       </c>
@@ -10119,7 +10136,7 @@
       <c r="AE93" s="50"/>
       <c r="AF93" s="50"/>
     </row>
-    <row r="94" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="40" t="s">
         <v>153</v>
       </c>
@@ -10204,7 +10221,7 @@
       <c r="AE94" s="50"/>
       <c r="AF94" s="50"/>
     </row>
-    <row r="95" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="40" t="s">
         <v>154</v>
       </c>
@@ -10289,7 +10306,7 @@
       <c r="AE95" s="50"/>
       <c r="AF95" s="50"/>
     </row>
-    <row r="96" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="40" t="s">
         <v>155</v>
       </c>
@@ -10374,7 +10391,7 @@
       <c r="AE96" s="50"/>
       <c r="AF96" s="50"/>
     </row>
-    <row r="97" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="40" t="s">
         <v>156</v>
       </c>
@@ -10459,7 +10476,7 @@
       <c r="AE97" s="50"/>
       <c r="AF97" s="50"/>
     </row>
-    <row r="98" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="40" t="s">
         <v>157</v>
       </c>
@@ -10544,7 +10561,7 @@
       <c r="AE98" s="50"/>
       <c r="AF98" s="50"/>
     </row>
-    <row r="99" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="40" t="s">
         <v>158</v>
       </c>
@@ -10629,7 +10646,7 @@
       <c r="AE99" s="50"/>
       <c r="AF99" s="50"/>
     </row>
-    <row r="100" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="40" t="s">
         <v>159</v>
       </c>
@@ -10714,7 +10731,7 @@
       <c r="AE100" s="50"/>
       <c r="AF100" s="50"/>
     </row>
-    <row r="101" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="40" t="s">
         <v>161</v>
       </c>
@@ -10799,7 +10816,7 @@
       <c r="AE101" s="50"/>
       <c r="AF101" s="50"/>
     </row>
-    <row r="102" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="40" t="s">
         <v>163</v>
       </c>
@@ -10884,7 +10901,7 @@
       <c r="AE102" s="50"/>
       <c r="AF102" s="50"/>
     </row>
-    <row r="103" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="40" t="s">
         <v>165</v>
       </c>
@@ -10969,7 +10986,7 @@
       <c r="AE103" s="50"/>
       <c r="AF103" s="50"/>
     </row>
-    <row r="104" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="40" t="s">
         <v>167</v>
       </c>
@@ -11054,7 +11071,7 @@
       <c r="AE104" s="50"/>
       <c r="AF104" s="50"/>
     </row>
-    <row r="105" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="40" t="s">
         <v>169</v>
       </c>
@@ -11139,7 +11156,7 @@
       <c r="AE105" s="50"/>
       <c r="AF105" s="50"/>
     </row>
-    <row r="106" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="40" t="s">
         <v>171</v>
       </c>
@@ -11224,7 +11241,7 @@
       <c r="AE106" s="50"/>
       <c r="AF106" s="50"/>
     </row>
-    <row r="107" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="40" t="s">
         <v>173</v>
       </c>
@@ -11309,7 +11326,7 @@
       <c r="AE107" s="50"/>
       <c r="AF107" s="50"/>
     </row>
-    <row r="108" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="40" t="s">
         <v>175</v>
       </c>
@@ -11394,7 +11411,7 @@
       <c r="AE108" s="50"/>
       <c r="AF108" s="50"/>
     </row>
-    <row r="109" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="40" t="s">
         <v>177</v>
       </c>
@@ -11479,7 +11496,7 @@
       <c r="AE109" s="50"/>
       <c r="AF109" s="50"/>
     </row>
-    <row r="110" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="40" t="s">
         <v>178</v>
       </c>
@@ -11564,7 +11581,7 @@
       <c r="AE110" s="50"/>
       <c r="AF110" s="50"/>
     </row>
-    <row r="111" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="40" t="s">
         <v>179</v>
       </c>
@@ -11649,7 +11666,7 @@
       <c r="AE111" s="50"/>
       <c r="AF111" s="50"/>
     </row>
-    <row r="112" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="40" t="s">
         <v>180</v>
       </c>
@@ -11734,7 +11751,7 @@
       <c r="AE112" s="50"/>
       <c r="AF112" s="50"/>
     </row>
-    <row r="113" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="40" t="s">
         <v>181</v>
       </c>
@@ -11819,7 +11836,7 @@
       <c r="AE113" s="50"/>
       <c r="AF113" s="50"/>
     </row>
-    <row r="114" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="40" t="s">
         <v>182</v>
       </c>
@@ -11904,7 +11921,7 @@
       <c r="AE114" s="50"/>
       <c r="AF114" s="50"/>
     </row>
-    <row r="115" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="40" t="s">
         <v>183</v>
       </c>
@@ -11989,7 +12006,7 @@
       <c r="AE115" s="50"/>
       <c r="AF115" s="50"/>
     </row>
-    <row r="116" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="40" t="s">
         <v>184</v>
       </c>
@@ -12074,7 +12091,7 @@
       <c r="AE116" s="50"/>
       <c r="AF116" s="50"/>
     </row>
-    <row r="117" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="40" t="s">
         <v>185</v>
       </c>
@@ -12159,7 +12176,7 @@
       <c r="AE117" s="50"/>
       <c r="AF117" s="50"/>
     </row>
-    <row r="118" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="40" t="s">
         <v>186</v>
       </c>
@@ -12244,7 +12261,7 @@
       <c r="AE118" s="50"/>
       <c r="AF118" s="50"/>
     </row>
-    <row r="119" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="40" t="s">
         <v>187</v>
       </c>
@@ -12330,7 +12347,7 @@
       <c r="AE119" s="50"/>
       <c r="AF119" s="50"/>
     </row>
-    <row r="120" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="40" t="s">
         <v>188</v>
       </c>
@@ -12416,7 +12433,7 @@
       <c r="AE120" s="50"/>
       <c r="AF120" s="50"/>
     </row>
-    <row r="121" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="40" t="s">
         <v>189</v>
       </c>
@@ -12501,7 +12518,7 @@
       <c r="AE121" s="50"/>
       <c r="AF121" s="50"/>
     </row>
-    <row r="122" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="40" t="s">
         <v>190</v>
       </c>
@@ -12586,7 +12603,7 @@
       <c r="AE122" s="50"/>
       <c r="AF122" s="50"/>
     </row>
-    <row r="123" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="40" t="s">
         <v>192</v>
       </c>
@@ -12671,7 +12688,7 @@
       <c r="AE123" s="50"/>
       <c r="AF123" s="50"/>
     </row>
-    <row r="124" spans="1:32" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:32" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="40" t="s">
         <v>194</v>
       </c>
@@ -12756,7 +12773,7 @@
       <c r="AE124" s="50"/>
       <c r="AF124" s="50"/>
     </row>
-    <row r="125" spans="1:32" s="50" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:32" s="50" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="40" t="s">
         <v>196</v>
       </c>
@@ -12839,7 +12856,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="126" spans="1:32" s="50" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:32" s="50" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="40" t="s">
         <v>197</v>
       </c>
@@ -12922,7 +12939,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="127" spans="1:32" s="50" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:32" s="50" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="40" t="s">
         <v>198</v>
       </c>
@@ -13005,7 +13022,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="128" spans="1:32" s="50" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:32" s="50" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="40" t="s">
         <v>228</v>
       </c>
@@ -13088,7 +13105,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="129" spans="1:255" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:255" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="40" t="s">
         <v>225</v>
       </c>
@@ -13173,7 +13190,7 @@
       <c r="AE129" s="50"/>
       <c r="AF129" s="50"/>
     </row>
-    <row r="130" spans="1:255" s="4" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:255" s="4" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="40" t="s">
         <v>226</v>
       </c>
@@ -13258,7 +13275,7 @@
       <c r="AE130" s="50"/>
       <c r="AF130" s="50"/>
     </row>
-    <row r="131" spans="1:255" s="18" customFormat="1" ht="38.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:255" s="18" customFormat="1" ht="38.450000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="40" t="s">
         <v>227</v>
       </c>
@@ -13567,7 +13584,7 @@
       <c r="IT131" s="4"/>
       <c r="IU131" s="4"/>
     </row>
-    <row r="132" spans="1:255" s="50" customFormat="1" ht="23.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:255" s="50" customFormat="1" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="12" t="s">
         <v>238</v>
       </c>
@@ -13600,7 +13617,7 @@
       <c r="AV132" s="61"/>
       <c r="AW132" s="61"/>
     </row>
-    <row r="133" spans="1:255" s="50" customFormat="1" ht="21.6" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:255" s="50" customFormat="1" ht="21" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A133" s="11" t="s">
         <v>240</v>
       </c>
@@ -13627,7 +13644,7 @@
       <c r="AS133" s="61"/>
       <c r="AT133" s="61"/>
     </row>
-    <row r="134" spans="1:255" s="50" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:255" s="50" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="56" t="s">
         <v>241</v>
       </c>
@@ -13654,7 +13671,7 @@
       <c r="AS134" s="61"/>
       <c r="AT134" s="61"/>
     </row>
-    <row r="135" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="56" t="s">
         <v>242</v>
       </c>
@@ -13681,7 +13698,7 @@
       <c r="AS135" s="61"/>
       <c r="AT135" s="61"/>
     </row>
-    <row r="136" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="41" t="s">
         <v>243</v>
       </c>
@@ -13708,7 +13725,7 @@
       <c r="AS136" s="61"/>
       <c r="AT136" s="61"/>
     </row>
-    <row r="137" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="41" t="s">
         <v>244</v>
       </c>
@@ -13735,7 +13752,7 @@
       <c r="AS137" s="61"/>
       <c r="AT137" s="61"/>
     </row>
-    <row r="138" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="41" t="s">
         <v>245</v>
       </c>
@@ -13762,7 +13779,7 @@
       <c r="AS138" s="61"/>
       <c r="AT138" s="61"/>
     </row>
-    <row r="139" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="41" t="s">
         <v>246</v>
       </c>
@@ -13789,7 +13806,7 @@
       <c r="AS139" s="61"/>
       <c r="AT139" s="61"/>
     </row>
-    <row r="140" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="41" t="s">
         <v>247</v>
       </c>
@@ -13816,7 +13833,7 @@
       <c r="AS140" s="61"/>
       <c r="AT140" s="61"/>
     </row>
-    <row r="141" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="41" t="s">
         <v>248</v>
       </c>
@@ -13843,7 +13860,7 @@
       <c r="AS141" s="61"/>
       <c r="AT141" s="61"/>
     </row>
-    <row r="142" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:255" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="41" t="s">
         <v>249</v>
       </c>
@@ -13870,9 +13887,9 @@
       <c r="AS142" s="61"/>
       <c r="AT142" s="61"/>
     </row>
-    <row r="143" spans="1:255" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:255" x14ac:dyDescent="0.3">
       <c r="A143" s="56" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="B143" s="51"/>
       <c r="C143" s="64"/>
@@ -13895,9 +13912,9 @@
       <c r="T143" s="5"/>
       <c r="U143" s="5"/>
     </row>
-    <row r="144" spans="1:255" s="53" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:255" s="53" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="56" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B144" s="51"/>
       <c r="C144" s="64"/>
@@ -13922,9 +13939,9 @@
       <c r="AS144" s="63"/>
       <c r="AT144" s="63"/>
     </row>
-    <row r="145" spans="1:46" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:46" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="56" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B145" s="66"/>
       <c r="C145" s="67"/>
@@ -13949,9 +13966,9 @@
       <c r="AS145" s="61"/>
       <c r="AT145" s="61"/>
     </row>
-    <row r="146" spans="1:46" s="53" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:46" s="53" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="56" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B146" s="51"/>
       <c r="C146" s="64"/>
@@ -13976,9 +13993,9 @@
       <c r="AS146" s="63"/>
       <c r="AT146" s="63"/>
     </row>
-    <row r="147" spans="1:46" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:46" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="56" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B147" s="51"/>
       <c r="C147" s="64"/>
@@ -14003,9 +14020,9 @@
       <c r="AS147" s="61"/>
       <c r="AT147" s="61"/>
     </row>
-    <row r="148" spans="1:46" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:46" s="50" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="56" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B148" s="51"/>
       <c r="C148" s="64"/>
@@ -14030,512 +14047,512 @@
       <c r="AS148" s="61"/>
       <c r="AT148" s="61"/>
     </row>
-    <row r="149" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:46" x14ac:dyDescent="0.3">
       <c r="D149" s="7"/>
       <c r="E149" s="7"/>
       <c r="F149" s="7"/>
       <c r="G149" s="47"/>
     </row>
-    <row r="150" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:46" x14ac:dyDescent="0.3">
       <c r="D150" s="7"/>
       <c r="E150" s="7"/>
       <c r="F150" s="7"/>
       <c r="G150" s="47"/>
     </row>
-    <row r="151" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:46" x14ac:dyDescent="0.3">
       <c r="D151" s="7"/>
       <c r="E151" s="7"/>
       <c r="F151" s="7"/>
       <c r="G151" s="47"/>
     </row>
-    <row r="152" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:46" x14ac:dyDescent="0.3">
       <c r="D152" s="7"/>
       <c r="E152" s="7"/>
       <c r="F152" s="7"/>
       <c r="G152" s="47"/>
     </row>
-    <row r="153" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="153" spans="1:46" x14ac:dyDescent="0.3">
       <c r="D153" s="7"/>
       <c r="E153" s="7"/>
       <c r="F153" s="7"/>
       <c r="G153" s="47"/>
     </row>
-    <row r="154" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="154" spans="1:46" x14ac:dyDescent="0.3">
       <c r="D154" s="7"/>
       <c r="E154" s="7"/>
       <c r="F154" s="7"/>
       <c r="G154" s="47"/>
     </row>
-    <row r="155" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="155" spans="1:46" x14ac:dyDescent="0.3">
       <c r="D155" s="7"/>
       <c r="E155" s="7"/>
       <c r="F155" s="7"/>
       <c r="G155" s="47"/>
     </row>
-    <row r="156" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="156" spans="1:46" x14ac:dyDescent="0.3">
       <c r="D156" s="7"/>
       <c r="E156" s="7"/>
       <c r="F156" s="7"/>
       <c r="G156" s="47"/>
     </row>
-    <row r="157" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="157" spans="1:46" x14ac:dyDescent="0.3">
       <c r="D157" s="7"/>
       <c r="E157" s="7"/>
       <c r="F157" s="7"/>
       <c r="G157" s="47"/>
     </row>
-    <row r="158" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="158" spans="1:46" x14ac:dyDescent="0.3">
       <c r="D158" s="7"/>
       <c r="E158" s="7"/>
       <c r="F158" s="7"/>
       <c r="G158" s="47"/>
     </row>
-    <row r="159" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="159" spans="1:46" x14ac:dyDescent="0.3">
       <c r="D159" s="7"/>
       <c r="E159" s="7"/>
       <c r="F159" s="7"/>
       <c r="G159" s="47"/>
     </row>
-    <row r="160" spans="1:46" x14ac:dyDescent="0.4">
+    <row r="160" spans="1:46" x14ac:dyDescent="0.3">
       <c r="D160" s="7"/>
       <c r="E160" s="7"/>
       <c r="F160" s="7"/>
       <c r="G160" s="47"/>
     </row>
-    <row r="161" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="161" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D161" s="7"/>
       <c r="E161" s="7"/>
       <c r="F161" s="7"/>
       <c r="G161" s="47"/>
     </row>
-    <row r="162" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="162" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D162" s="7"/>
       <c r="E162" s="7"/>
       <c r="F162" s="7"/>
       <c r="G162" s="47"/>
     </row>
-    <row r="163" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="163" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D163" s="7"/>
       <c r="E163" s="7"/>
       <c r="F163" s="7"/>
       <c r="G163" s="47"/>
     </row>
-    <row r="164" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="164" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D164" s="7"/>
       <c r="E164" s="7"/>
       <c r="F164" s="7"/>
       <c r="G164" s="47"/>
     </row>
-    <row r="165" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="165" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D165" s="7"/>
       <c r="E165" s="7"/>
       <c r="F165" s="7"/>
       <c r="G165" s="47"/>
     </row>
-    <row r="166" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="166" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D166" s="7"/>
       <c r="E166" s="7"/>
       <c r="F166" s="7"/>
       <c r="G166" s="47"/>
     </row>
-    <row r="167" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="167" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D167" s="7"/>
       <c r="E167" s="7"/>
       <c r="F167" s="7"/>
       <c r="G167" s="47"/>
     </row>
-    <row r="168" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="168" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D168" s="7"/>
       <c r="E168" s="7"/>
       <c r="F168" s="7"/>
       <c r="G168" s="47"/>
     </row>
-    <row r="169" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="169" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D169" s="7"/>
       <c r="E169" s="7"/>
       <c r="F169" s="7"/>
       <c r="G169" s="47"/>
     </row>
-    <row r="170" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="170" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D170" s="7"/>
       <c r="E170" s="7"/>
       <c r="F170" s="7"/>
       <c r="G170" s="47"/>
     </row>
-    <row r="171" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="171" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D171" s="7"/>
       <c r="E171" s="7"/>
       <c r="F171" s="7"/>
       <c r="G171" s="47"/>
     </row>
-    <row r="172" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="172" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D172" s="7"/>
       <c r="E172" s="7"/>
       <c r="F172" s="7"/>
       <c r="G172" s="47"/>
     </row>
-    <row r="173" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="173" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D173" s="7"/>
       <c r="E173" s="7"/>
       <c r="F173" s="7"/>
       <c r="G173" s="47"/>
     </row>
-    <row r="174" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="174" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D174" s="7"/>
       <c r="E174" s="7"/>
       <c r="F174" s="7"/>
       <c r="G174" s="47"/>
     </row>
-    <row r="175" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="175" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D175" s="7"/>
       <c r="E175" s="7"/>
       <c r="F175" s="7"/>
       <c r="G175" s="47"/>
     </row>
-    <row r="176" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="176" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D176" s="7"/>
       <c r="E176" s="7"/>
       <c r="F176" s="7"/>
       <c r="G176" s="47"/>
     </row>
-    <row r="177" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="177" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D177" s="7"/>
       <c r="E177" s="7"/>
       <c r="F177" s="7"/>
       <c r="G177" s="47"/>
     </row>
-    <row r="178" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="178" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D178" s="7"/>
       <c r="E178" s="7"/>
       <c r="F178" s="7"/>
       <c r="G178" s="47"/>
     </row>
-    <row r="179" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="179" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D179" s="7"/>
       <c r="E179" s="7"/>
       <c r="F179" s="7"/>
       <c r="G179" s="47"/>
     </row>
-    <row r="180" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="180" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D180" s="7"/>
       <c r="E180" s="7"/>
       <c r="F180" s="7"/>
       <c r="G180" s="47"/>
     </row>
-    <row r="181" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="181" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D181" s="7"/>
       <c r="E181" s="7"/>
       <c r="F181" s="7"/>
       <c r="G181" s="47"/>
     </row>
-    <row r="182" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="182" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D182" s="7"/>
       <c r="E182" s="7"/>
       <c r="F182" s="7"/>
       <c r="G182" s="47"/>
     </row>
-    <row r="183" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="183" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D183" s="7"/>
       <c r="E183" s="7"/>
       <c r="F183" s="7"/>
       <c r="G183" s="47"/>
     </row>
-    <row r="184" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="184" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D184" s="7"/>
       <c r="E184" s="7"/>
       <c r="F184" s="7"/>
       <c r="G184" s="47"/>
     </row>
-    <row r="185" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="185" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D185" s="7"/>
       <c r="E185" s="7"/>
       <c r="F185" s="7"/>
       <c r="G185" s="47"/>
     </row>
-    <row r="186" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="186" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D186" s="7"/>
       <c r="E186" s="7"/>
       <c r="F186" s="7"/>
       <c r="G186" s="47"/>
     </row>
-    <row r="187" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="187" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D187" s="7"/>
       <c r="E187" s="7"/>
       <c r="F187" s="7"/>
       <c r="G187" s="47"/>
     </row>
-    <row r="188" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="188" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D188" s="7"/>
       <c r="E188" s="7"/>
       <c r="F188" s="7"/>
       <c r="G188" s="47"/>
     </row>
-    <row r="189" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="189" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D189" s="7"/>
       <c r="E189" s="7"/>
       <c r="F189" s="7"/>
       <c r="G189" s="47"/>
     </row>
-    <row r="190" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="190" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D190" s="7"/>
       <c r="E190" s="7"/>
       <c r="F190" s="7"/>
       <c r="G190" s="47"/>
     </row>
-    <row r="191" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="191" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
       <c r="F191" s="7"/>
       <c r="G191" s="47"/>
     </row>
-    <row r="192" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="192" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D192" s="7"/>
       <c r="E192" s="7"/>
       <c r="F192" s="7"/>
       <c r="G192" s="47"/>
     </row>
-    <row r="193" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="193" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D193" s="7"/>
       <c r="E193" s="7"/>
       <c r="F193" s="7"/>
       <c r="G193" s="47"/>
     </row>
-    <row r="194" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="194" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D194" s="7"/>
       <c r="E194" s="7"/>
       <c r="F194" s="7"/>
       <c r="G194" s="47"/>
     </row>
-    <row r="195" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="195" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D195" s="7"/>
       <c r="E195" s="7"/>
       <c r="F195" s="7"/>
       <c r="G195" s="47"/>
     </row>
-    <row r="196" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="196" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D196" s="7"/>
       <c r="E196" s="7"/>
       <c r="F196" s="7"/>
       <c r="G196" s="47"/>
     </row>
-    <row r="197" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="197" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D197" s="7"/>
       <c r="E197" s="7"/>
       <c r="F197" s="7"/>
       <c r="G197" s="47"/>
     </row>
-    <row r="198" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="198" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D198" s="7"/>
       <c r="E198" s="7"/>
       <c r="F198" s="7"/>
       <c r="G198" s="47"/>
     </row>
-    <row r="199" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="199" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D199" s="7"/>
       <c r="E199" s="7"/>
       <c r="F199" s="7"/>
       <c r="G199" s="47"/>
     </row>
-    <row r="200" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="200" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D200" s="7"/>
       <c r="E200" s="7"/>
       <c r="F200" s="7"/>
       <c r="G200" s="47"/>
     </row>
-    <row r="201" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="201" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D201" s="7"/>
       <c r="E201" s="7"/>
       <c r="F201" s="7"/>
       <c r="G201" s="47"/>
     </row>
-    <row r="202" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="202" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D202" s="7"/>
       <c r="E202" s="7"/>
       <c r="F202" s="7"/>
       <c r="G202" s="47"/>
     </row>
-    <row r="203" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="203" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D203" s="7"/>
       <c r="E203" s="7"/>
       <c r="F203" s="7"/>
       <c r="G203" s="47"/>
     </row>
-    <row r="204" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="204" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D204" s="7"/>
       <c r="E204" s="7"/>
       <c r="F204" s="7"/>
       <c r="G204" s="47"/>
     </row>
-    <row r="205" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="205" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D205" s="7"/>
       <c r="E205" s="7"/>
       <c r="F205" s="7"/>
       <c r="G205" s="47"/>
     </row>
-    <row r="206" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="206" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D206" s="7"/>
       <c r="E206" s="7"/>
       <c r="F206" s="7"/>
       <c r="G206" s="47"/>
     </row>
-    <row r="207" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="207" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D207" s="7"/>
       <c r="E207" s="7"/>
       <c r="F207" s="7"/>
       <c r="G207" s="47"/>
     </row>
-    <row r="208" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="208" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D208" s="7"/>
       <c r="E208" s="7"/>
       <c r="F208" s="7"/>
       <c r="G208" s="47"/>
     </row>
-    <row r="209" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="209" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D209" s="7"/>
       <c r="E209" s="7"/>
       <c r="F209" s="7"/>
       <c r="G209" s="47"/>
     </row>
-    <row r="210" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="210" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D210" s="7"/>
       <c r="E210" s="7"/>
       <c r="F210" s="7"/>
       <c r="G210" s="47"/>
     </row>
-    <row r="211" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="211" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D211" s="7"/>
       <c r="E211" s="7"/>
       <c r="F211" s="7"/>
       <c r="G211" s="47"/>
     </row>
-    <row r="212" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="212" spans="4:7" x14ac:dyDescent="0.3">
       <c r="F212" s="7"/>
       <c r="G212" s="47"/>
     </row>
-    <row r="213" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="213" spans="4:7" x14ac:dyDescent="0.3">
       <c r="G213" s="47"/>
     </row>
-    <row r="214" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="214" spans="4:7" x14ac:dyDescent="0.3">
       <c r="G214" s="47"/>
     </row>
-    <row r="215" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="215" spans="4:7" x14ac:dyDescent="0.3">
       <c r="G215" s="47"/>
     </row>
-    <row r="216" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="216" spans="4:7" x14ac:dyDescent="0.3">
       <c r="G216" s="47"/>
     </row>
-    <row r="221" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="221" spans="4:7" x14ac:dyDescent="0.3">
       <c r="G221" s="5"/>
     </row>
-    <row r="222" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="222" spans="4:7" x14ac:dyDescent="0.3">
       <c r="G222" s="5"/>
     </row>
-    <row r="223" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="223" spans="4:7" x14ac:dyDescent="0.3">
       <c r="G223" s="5"/>
     </row>
-    <row r="224" spans="4:7" x14ac:dyDescent="0.4">
+    <row r="224" spans="4:7" x14ac:dyDescent="0.3">
       <c r="G224" s="5"/>
     </row>
-    <row r="225" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="225" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G225" s="5"/>
     </row>
-    <row r="226" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="226" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G226" s="5"/>
     </row>
-    <row r="227" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="227" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G227" s="5"/>
     </row>
-    <row r="228" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="228" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G228" s="5"/>
     </row>
-    <row r="229" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="229" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G229" s="5"/>
     </row>
-    <row r="230" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="230" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G230" s="5"/>
     </row>
-    <row r="231" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="231" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G231" s="5"/>
     </row>
-    <row r="232" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="232" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G232" s="5"/>
     </row>
-    <row r="233" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="233" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G233" s="5"/>
     </row>
-    <row r="234" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="234" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G234" s="5"/>
     </row>
-    <row r="235" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="235" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G235" s="5"/>
     </row>
-    <row r="236" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="236" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G236" s="5"/>
     </row>
-    <row r="237" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="237" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G237" s="5"/>
     </row>
-    <row r="238" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="238" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G238" s="5"/>
     </row>
-    <row r="239" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="239" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G239" s="5"/>
     </row>
-    <row r="240" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="240" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G240" s="5"/>
     </row>
-    <row r="241" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="241" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G241" s="5"/>
     </row>
-    <row r="242" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="242" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G242" s="5"/>
     </row>
-    <row r="243" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="243" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G243" s="5"/>
     </row>
-    <row r="244" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="244" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G244" s="5"/>
     </row>
-    <row r="245" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="245" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G245" s="5"/>
     </row>
-    <row r="246" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="246" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G246" s="5"/>
     </row>
-    <row r="247" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="247" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G247" s="5"/>
     </row>
-    <row r="248" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="248" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G248" s="5"/>
     </row>
-    <row r="249" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="249" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G249" s="5"/>
     </row>
-    <row r="250" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="250" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G250" s="5"/>
     </row>
-    <row r="251" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="251" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G251" s="5"/>
     </row>
-    <row r="252" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="252" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G252" s="5"/>
     </row>
-    <row r="253" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="253" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G253" s="5"/>
     </row>
-    <row r="254" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="254" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G254" s="5"/>
     </row>
-    <row r="255" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="255" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G255" s="5"/>
     </row>
-    <row r="256" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="256" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G256" s="5"/>
     </row>
-    <row r="1892" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="1892" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G1892" s="5"/>
     </row>
-    <row r="1893" spans="7:7" x14ac:dyDescent="0.4">
+    <row r="1893" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G1893" s="5"/>
     </row>
   </sheetData>
@@ -14685,13 +14702,12 @@
   <phoneticPr fontId="20" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094499" right="0.23622047244094499" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
-  <pageSetup paperSize="9" scale="52" firstPageNumber="2" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="17" firstPageNumber="2" fitToHeight="0" orientation="portrait" useFirstPageNumber="1" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0">
     <oddFooter>&amp;C&amp;10&amp;P</oddFooter>
   </headerFooter>
-  <rowBreaks count="2" manualBreakCount="2">
-    <brk id="73" max="20" man="1"/>
-    <brk id="105" max="20" man="1"/>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="114" max="20" man="1"/>
   </rowBreaks>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update last 5 years report
1. add last 5 years report function
2. rollback dailytrans report template.xlsx 珍珠芭 -> 珍珠拔
3. update requirements.txt pyyaml>=5.3.1 for security issue
</commit_message>
<xml_diff>
--- a/src/apps/dailytrans/reports/template.xlsx
+++ b/src/apps/dailytrans/reports/template.xlsx
@@ -581,9 +581,6 @@
   </si>
   <si>
     <t>60</t>
-  </si>
-  <si>
-    <t>珍珠芭</t>
   </si>
   <si>
     <t>61</t>
@@ -1453,6 +1450,10 @@
   <si>
     <t>番荔枝
 (大目)</t>
+    <phoneticPr fontId="26" type="noConversion"/>
+  </si>
+  <si>
+    <t>珍珠拔</t>
     <phoneticPr fontId="26" type="noConversion"/>
   </si>
 </sst>
@@ -2023,36 +2024,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="21" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2091,6 +2062,36 @@
     </xf>
     <xf numFmtId="179" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="21" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2468,8 +2469,8 @@
   <dimension ref="A1:AMJ256"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63:C63"/>
+      <pane ySplit="8" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B80" sqref="B80:C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -2503,35 +2504,35 @@
       <c r="F1" s="8"/>
       <c r="G1" s="9"/>
       <c r="H1" s="10"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
       <c r="M1" s="11"/>
       <c r="N1" s="11"/>
     </row>
     <row r="2" spans="1:30" s="12" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="88"/>
-      <c r="S2" s="88"/>
-      <c r="T2" s="88"/>
-      <c r="U2" s="88"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
     </row>
     <row r="3" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="13"/>
@@ -2580,8 +2581,8 @@
       <c r="G5" s="20"/>
       <c r="H5" s="21"/>
       <c r="I5" s="22"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
       <c r="L5" s="21"/>
       <c r="M5" s="23"/>
       <c r="N5" s="23"/>
@@ -2590,41 +2591,41 @@
       <c r="S5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="T5" s="90" t="s">
+      <c r="T5" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="U5" s="90"/>
+      <c r="U5" s="80"/>
     </row>
     <row r="6" spans="1:30" s="12" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="91" t="s">
+      <c r="A6" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="94" t="s">
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="95" t="s">
+      <c r="G6" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="91" t="s">
+      <c r="H6" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
-      <c r="O6" s="91"/>
-      <c r="P6" s="91"/>
-      <c r="Q6" s="91"/>
-      <c r="R6" s="91"/>
-      <c r="S6" s="91"/>
-      <c r="T6" s="91"/>
-      <c r="U6" s="91"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="81"/>
+      <c r="O6" s="81"/>
+      <c r="P6" s="81"/>
+      <c r="Q6" s="81"/>
+      <c r="R6" s="81"/>
+      <c r="S6" s="81"/>
+      <c r="T6" s="81"/>
+      <c r="U6" s="81"/>
       <c r="V6" s="1"/>
       <c r="W6" s="28"/>
       <c r="X6" s="28"/>
@@ -2636,36 +2637,36 @@
       <c r="AD6" s="28"/>
     </row>
     <row r="7" spans="1:30" s="12" customFormat="1" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="91"/>
-      <c r="B7" s="91"/>
-      <c r="C7" s="91"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="96" t="s">
+      <c r="A7" s="81"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="86" t="s">
         <v>7</v>
       </c>
       <c r="I7" s="29"/>
       <c r="J7" s="29"/>
       <c r="K7" s="29"/>
-      <c r="L7" s="97" t="s">
-        <v>247</v>
-      </c>
-      <c r="M7" s="98" t="s">
+      <c r="L7" s="87" t="s">
+        <v>246</v>
+      </c>
+      <c r="M7" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="98"/>
-      <c r="O7" s="98"/>
-      <c r="P7" s="98"/>
-      <c r="Q7" s="98"/>
-      <c r="R7" s="98"/>
-      <c r="S7" s="98"/>
-      <c r="T7" s="99" t="s">
+      <c r="N7" s="88"/>
+      <c r="O7" s="88"/>
+      <c r="P7" s="88"/>
+      <c r="Q7" s="88"/>
+      <c r="R7" s="88"/>
+      <c r="S7" s="88"/>
+      <c r="T7" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="U7" s="99"/>
-      <c r="V7" s="84"/>
+      <c r="U7" s="89"/>
+      <c r="V7" s="90"/>
       <c r="W7" s="30"/>
       <c r="X7" s="30"/>
       <c r="Y7" s="30"/>
@@ -2676,14 +2677,14 @@
       <c r="AD7" s="30"/>
     </row>
     <row r="8" spans="1:30" s="12" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="91"/>
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="95"/>
-      <c r="H8" s="96"/>
+      <c r="A8" s="81"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="86"/>
       <c r="I8" s="31" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -2696,9 +2697,9 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="L8" s="97"/>
+      <c r="L8" s="87"/>
       <c r="M8" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N8" s="32" t="s">
         <v>10</v>
@@ -2722,9 +2723,9 @@
         <v>11</v>
       </c>
       <c r="U8" s="33" t="s">
-        <v>249</v>
-      </c>
-      <c r="V8" s="84"/>
+        <v>248</v>
+      </c>
+      <c r="V8" s="90"/>
       <c r="W8" s="34" t="s">
         <v>12</v>
       </c>
@@ -2754,13 +2755,13 @@
       <c r="A9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="77"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="86" t="s">
+      <c r="C9" s="91"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="93" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="37" t="s">
@@ -2837,13 +2838,13 @@
       <c r="A10" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="92"/>
       <c r="G10" s="37" t="s">
         <v>15</v>
       </c>
@@ -2918,10 +2919,10 @@
       <c r="A11" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="77"/>
+      <c r="C11" s="91"/>
       <c r="D11" s="36" t="s">
         <v>15</v>
       </c>
@@ -3005,10 +3006,10 @@
       <c r="A12" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="77" t="s">
+      <c r="B12" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="77"/>
+      <c r="C12" s="91"/>
       <c r="D12" s="36" t="s">
         <v>15</v>
       </c>
@@ -3092,10 +3093,10 @@
       <c r="A13" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="77"/>
+      <c r="C13" s="91"/>
       <c r="D13" s="36" t="s">
         <v>15</v>
       </c>
@@ -3179,10 +3180,10 @@
       <c r="A14" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="78" t="s">
+      <c r="B14" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="78"/>
+      <c r="C14" s="94"/>
       <c r="D14" s="43"/>
       <c r="E14" s="43"/>
       <c r="F14" s="36" t="s">
@@ -3263,10 +3264,10 @@
       <c r="A15" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="78" t="s">
+      <c r="B15" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="78"/>
+      <c r="C15" s="94"/>
       <c r="D15" s="43"/>
       <c r="E15" s="43"/>
       <c r="F15" s="36" t="s">
@@ -3346,10 +3347,10 @@
       <c r="A16" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="78" t="s">
+      <c r="B16" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="78"/>
+      <c r="C16" s="94"/>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
       <c r="F16" s="36" t="s">
@@ -3429,10 +3430,10 @@
       <c r="A17" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="78"/>
+      <c r="C17" s="94"/>
       <c r="D17" s="43"/>
       <c r="E17" s="43"/>
       <c r="F17" s="36" t="s">
@@ -3512,10 +3513,10 @@
       <c r="A18" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="83"/>
+      <c r="C18" s="95"/>
       <c r="D18" s="43"/>
       <c r="E18" s="43"/>
       <c r="F18" s="36" t="s">
@@ -3595,10 +3596,10 @@
       <c r="A19" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="78" t="s">
+      <c r="B19" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="78"/>
+      <c r="C19" s="94"/>
       <c r="D19" s="43"/>
       <c r="E19" s="43"/>
       <c r="F19" s="36" t="s">
@@ -3678,10 +3679,10 @@
       <c r="A20" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="78" t="s">
+      <c r="B20" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="78"/>
+      <c r="C20" s="94"/>
       <c r="D20" s="43"/>
       <c r="E20" s="43"/>
       <c r="F20" s="36" t="s">
@@ -3761,10 +3762,10 @@
       <c r="A21" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="78" t="s">
+      <c r="B21" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="78"/>
+      <c r="C21" s="94"/>
       <c r="D21" s="43"/>
       <c r="E21" s="43"/>
       <c r="F21" s="36" t="s">
@@ -3844,10 +3845,10 @@
       <c r="A22" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="78" t="s">
+      <c r="B22" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="78"/>
+      <c r="C22" s="94"/>
       <c r="D22" s="43"/>
       <c r="E22" s="43"/>
       <c r="F22" s="36" t="s">
@@ -3927,10 +3928,10 @@
       <c r="A23" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="78" t="s">
+      <c r="B23" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="78"/>
+      <c r="C23" s="94"/>
       <c r="D23" s="43"/>
       <c r="E23" s="43"/>
       <c r="F23" s="36" t="s">
@@ -4010,10 +4011,10 @@
       <c r="A24" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="78" t="s">
+      <c r="B24" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="78"/>
+      <c r="C24" s="94"/>
       <c r="D24" s="43"/>
       <c r="E24" s="43"/>
       <c r="F24" s="36" t="s">
@@ -4093,10 +4094,10 @@
       <c r="A25" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="83" t="s">
+      <c r="B25" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="83"/>
+      <c r="C25" s="95"/>
       <c r="D25" s="43"/>
       <c r="E25" s="43"/>
       <c r="F25" s="36" t="s">
@@ -4176,10 +4177,10 @@
       <c r="A26" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="78" t="s">
+      <c r="B26" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="78"/>
+      <c r="C26" s="94"/>
       <c r="D26" s="43"/>
       <c r="E26" s="43"/>
       <c r="F26" s="36" t="s">
@@ -4259,10 +4260,10 @@
       <c r="A27" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="78" t="s">
+      <c r="B27" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="78"/>
+      <c r="C27" s="94"/>
       <c r="D27" s="43"/>
       <c r="E27" s="43"/>
       <c r="F27" s="36" t="s">
@@ -4342,10 +4343,10 @@
       <c r="A28" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="78" t="s">
+      <c r="B28" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="78"/>
+      <c r="C28" s="94"/>
       <c r="D28" s="43"/>
       <c r="E28" s="43"/>
       <c r="F28" s="36" t="s">
@@ -4425,10 +4426,10 @@
       <c r="A29" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="83" t="s">
+      <c r="B29" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="83"/>
+      <c r="C29" s="95"/>
       <c r="D29" s="43"/>
       <c r="E29" s="43"/>
       <c r="F29" s="36" t="s">
@@ -4509,10 +4510,10 @@
       <c r="A30" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="83" t="s">
+      <c r="B30" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="83"/>
+      <c r="C30" s="95"/>
       <c r="D30" s="43"/>
       <c r="E30" s="43"/>
       <c r="F30" s="36" t="s">
@@ -4593,10 +4594,10 @@
       <c r="A31" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="78" t="s">
+      <c r="B31" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="78"/>
+      <c r="C31" s="94"/>
       <c r="D31" s="43"/>
       <c r="E31" s="43"/>
       <c r="F31" s="36" t="s">
@@ -4676,10 +4677,10 @@
       <c r="A32" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="78" t="s">
+      <c r="B32" s="94" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="78"/>
+      <c r="C32" s="94"/>
       <c r="D32" s="43"/>
       <c r="E32" s="43"/>
       <c r="F32" s="36" t="s">
@@ -4759,10 +4760,10 @@
       <c r="A33" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="78" t="s">
+      <c r="B33" s="94" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="78"/>
+      <c r="C33" s="94"/>
       <c r="D33" s="45"/>
       <c r="E33" s="45"/>
       <c r="F33" s="36" t="s">
@@ -4843,10 +4844,10 @@
       <c r="A34" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="78" t="s">
+      <c r="B34" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="78"/>
+      <c r="C34" s="94"/>
       <c r="D34" s="45"/>
       <c r="E34" s="45"/>
       <c r="F34" s="36" t="s">
@@ -4926,10 +4927,10 @@
       <c r="A35" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="78" t="s">
+      <c r="B35" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="78"/>
+      <c r="C35" s="94"/>
       <c r="D35" s="45"/>
       <c r="E35" s="45"/>
       <c r="F35" s="36" t="s">
@@ -5009,10 +5010,10 @@
       <c r="A36" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="78" t="s">
+      <c r="B36" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="78"/>
+      <c r="C36" s="94"/>
       <c r="D36" s="45"/>
       <c r="E36" s="45"/>
       <c r="F36" s="36" t="s">
@@ -5092,10 +5093,10 @@
       <c r="A37" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="78" t="s">
+      <c r="B37" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="78"/>
+      <c r="C37" s="94"/>
       <c r="D37" s="45"/>
       <c r="E37" s="45"/>
       <c r="F37" s="36" t="s">
@@ -5175,10 +5176,10 @@
       <c r="A38" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="78" t="s">
+      <c r="B38" s="94" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="78"/>
+      <c r="C38" s="94"/>
       <c r="D38" s="45"/>
       <c r="E38" s="45"/>
       <c r="F38" s="36" t="s">
@@ -5258,10 +5259,10 @@
       <c r="A39" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="78" t="s">
+      <c r="B39" s="94" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="78"/>
+      <c r="C39" s="94"/>
       <c r="D39" s="45"/>
       <c r="E39" s="45"/>
       <c r="F39" s="36" t="s">
@@ -5341,10 +5342,10 @@
       <c r="A40" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="78" t="s">
+      <c r="B40" s="94" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="78"/>
+      <c r="C40" s="94"/>
       <c r="D40" s="45"/>
       <c r="E40" s="45"/>
       <c r="F40" s="36" t="s">
@@ -5424,10 +5425,10 @@
       <c r="A41" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="78" t="s">
+      <c r="B41" s="94" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="78"/>
+      <c r="C41" s="94"/>
       <c r="D41" s="45"/>
       <c r="E41" s="45"/>
       <c r="F41" s="36" t="s">
@@ -5507,10 +5508,10 @@
       <c r="A42" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="78" t="s">
+      <c r="B42" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="78"/>
+      <c r="C42" s="94"/>
       <c r="D42" s="45"/>
       <c r="E42" s="45"/>
       <c r="F42" s="36" t="s">
@@ -5591,10 +5592,10 @@
       <c r="A43" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="82" t="s">
+      <c r="B43" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="82"/>
+      <c r="C43" s="96"/>
       <c r="D43" s="45"/>
       <c r="E43" s="45"/>
       <c r="F43" s="36" t="s">
@@ -5674,10 +5675,10 @@
       <c r="A44" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="82" t="s">
+      <c r="B44" s="96" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="82"/>
+      <c r="C44" s="96"/>
       <c r="D44" s="45"/>
       <c r="E44" s="45"/>
       <c r="F44" s="36" t="s">
@@ -5757,10 +5758,10 @@
       <c r="A45" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="78" t="s">
+      <c r="B45" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="78"/>
+      <c r="C45" s="94"/>
       <c r="D45" s="45"/>
       <c r="E45" s="45"/>
       <c r="F45" s="36" t="s">
@@ -5840,10 +5841,10 @@
       <c r="A46" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="78" t="s">
+      <c r="B46" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="78"/>
+      <c r="C46" s="94"/>
       <c r="D46" s="45"/>
       <c r="E46" s="45"/>
       <c r="F46" s="36" t="s">
@@ -5923,10 +5924,10 @@
       <c r="A47" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="78" t="s">
+      <c r="B47" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C47" s="78"/>
+      <c r="C47" s="94"/>
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
       <c r="F47" s="36" t="s">
@@ -6006,10 +6007,10 @@
       <c r="A48" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="78" t="s">
+      <c r="B48" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="78"/>
+      <c r="C48" s="94"/>
       <c r="D48" s="45"/>
       <c r="E48" s="45"/>
       <c r="F48" s="36" t="s">
@@ -6089,10 +6090,10 @@
       <c r="A49" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="78" t="s">
+      <c r="B49" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C49" s="78"/>
+      <c r="C49" s="94"/>
       <c r="D49" s="45"/>
       <c r="E49" s="45"/>
       <c r="F49" s="36" t="s">
@@ -6172,10 +6173,10 @@
       <c r="A50" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="78" t="s">
+      <c r="B50" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C50" s="78"/>
+      <c r="C50" s="94"/>
       <c r="D50" s="45"/>
       <c r="E50" s="45"/>
       <c r="F50" s="36" t="s">
@@ -6255,10 +6256,10 @@
       <c r="A51" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="78" t="s">
+      <c r="B51" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C51" s="78"/>
+      <c r="C51" s="94"/>
       <c r="D51" s="45"/>
       <c r="E51" s="45"/>
       <c r="F51" s="36" t="s">
@@ -6338,10 +6339,10 @@
       <c r="A52" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="78" t="s">
+      <c r="B52" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="78"/>
+      <c r="C52" s="94"/>
       <c r="D52" s="45"/>
       <c r="E52" s="45"/>
       <c r="F52" s="36" t="s">
@@ -6421,10 +6422,10 @@
       <c r="A53" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="78" t="s">
+      <c r="B53" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="78"/>
+      <c r="C53" s="94"/>
       <c r="D53" s="45"/>
       <c r="E53" s="45"/>
       <c r="F53" s="36" t="s">
@@ -6504,10 +6505,10 @@
       <c r="A54" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="B54" s="78" t="s">
+      <c r="B54" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="78"/>
+      <c r="C54" s="94"/>
       <c r="D54" s="45"/>
       <c r="E54" s="45"/>
       <c r="F54" s="36" t="s">
@@ -6587,10 +6588,10 @@
       <c r="A55" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="B55" s="78" t="s">
+      <c r="B55" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C55" s="78"/>
+      <c r="C55" s="94"/>
       <c r="D55" s="45"/>
       <c r="E55" s="45"/>
       <c r="F55" s="36" t="s">
@@ -6670,10 +6671,10 @@
       <c r="A56" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="B56" s="78" t="s">
+      <c r="B56" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="C56" s="78"/>
+      <c r="C56" s="94"/>
       <c r="D56" s="45"/>
       <c r="E56" s="45"/>
       <c r="F56" s="36" t="s">
@@ -6753,10 +6754,10 @@
       <c r="A57" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="B57" s="78" t="s">
+      <c r="B57" s="94" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="78"/>
+      <c r="C57" s="94"/>
       <c r="D57" s="45"/>
       <c r="E57" s="45"/>
       <c r="F57" s="36" t="s">
@@ -6836,10 +6837,10 @@
       <c r="A58" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="B58" s="78" t="s">
+      <c r="B58" s="94" t="s">
         <v>104</v>
       </c>
-      <c r="C58" s="78"/>
+      <c r="C58" s="94"/>
       <c r="D58" s="45"/>
       <c r="E58" s="45"/>
       <c r="F58" s="36" t="s">
@@ -6919,10 +6920,10 @@
       <c r="A59" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="B59" s="78" t="s">
+      <c r="B59" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="C59" s="78"/>
+      <c r="C59" s="94"/>
       <c r="D59" s="45"/>
       <c r="E59" s="45"/>
       <c r="F59" s="36" t="s">
@@ -7002,10 +7003,10 @@
       <c r="A60" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="B60" s="78" t="s">
+      <c r="B60" s="94" t="s">
         <v>108</v>
       </c>
-      <c r="C60" s="78"/>
+      <c r="C60" s="94"/>
       <c r="D60" s="45"/>
       <c r="E60" s="45"/>
       <c r="F60" s="36" t="s">
@@ -7085,10 +7086,10 @@
       <c r="A61" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="B61" s="78" t="s">
+      <c r="B61" s="94" t="s">
         <v>110</v>
       </c>
-      <c r="C61" s="78"/>
+      <c r="C61" s="94"/>
       <c r="D61" s="45"/>
       <c r="E61" s="45"/>
       <c r="F61" s="36" t="s">
@@ -7168,10 +7169,10 @@
       <c r="A62" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="B62" s="78" t="s">
+      <c r="B62" s="94" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="78"/>
+      <c r="C62" s="94"/>
       <c r="D62" s="45"/>
       <c r="E62" s="45"/>
       <c r="F62" s="36" t="s">
@@ -7252,10 +7253,10 @@
       <c r="A63" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="B63" s="78" t="s">
-        <v>253</v>
-      </c>
-      <c r="C63" s="78"/>
+      <c r="B63" s="94" t="s">
+        <v>252</v>
+      </c>
+      <c r="C63" s="94"/>
       <c r="D63" s="45"/>
       <c r="E63" s="45"/>
       <c r="F63" s="36" t="s">
@@ -7335,10 +7336,10 @@
       <c r="A64" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="B64" s="78" t="s">
+      <c r="B64" s="94" t="s">
         <v>115</v>
       </c>
-      <c r="C64" s="78"/>
+      <c r="C64" s="94"/>
       <c r="D64" s="45"/>
       <c r="E64" s="45"/>
       <c r="F64" s="36" t="s">
@@ -7419,10 +7420,10 @@
       <c r="A65" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="B65" s="78" t="s">
+      <c r="B65" s="94" t="s">
         <v>117</v>
       </c>
-      <c r="C65" s="78"/>
+      <c r="C65" s="94"/>
       <c r="D65" s="45"/>
       <c r="E65" s="45"/>
       <c r="F65" s="36" t="s">
@@ -7502,10 +7503,10 @@
       <c r="A66" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="78" t="s">
+      <c r="B66" s="94" t="s">
         <v>119</v>
       </c>
-      <c r="C66" s="78"/>
+      <c r="C66" s="94"/>
       <c r="D66" s="45"/>
       <c r="E66" s="45"/>
       <c r="F66" s="36" t="s">
@@ -7586,10 +7587,10 @@
       <c r="A67" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="B67" s="78" t="s">
+      <c r="B67" s="94" t="s">
         <v>121</v>
       </c>
-      <c r="C67" s="78"/>
+      <c r="C67" s="94"/>
       <c r="D67" s="45"/>
       <c r="E67" s="45"/>
       <c r="F67" s="36" t="s">
@@ -7669,10 +7670,10 @@
       <c r="A68" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B68" s="78" t="s">
+      <c r="B68" s="94" t="s">
         <v>123</v>
       </c>
-      <c r="C68" s="78"/>
+      <c r="C68" s="94"/>
       <c r="D68" s="45"/>
       <c r="E68" s="45"/>
       <c r="F68" s="36" t="s">
@@ -7752,10 +7753,10 @@
       <c r="A69" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="B69" s="78" t="s">
+      <c r="B69" s="94" t="s">
         <v>125</v>
       </c>
-      <c r="C69" s="78"/>
+      <c r="C69" s="94"/>
       <c r="D69" s="45"/>
       <c r="E69" s="45"/>
       <c r="F69" s="36" t="s">
@@ -7836,10 +7837,10 @@
       <c r="A70" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="B70" s="78" t="s">
+      <c r="B70" s="94" t="s">
         <v>127</v>
       </c>
-      <c r="C70" s="78"/>
+      <c r="C70" s="94"/>
       <c r="D70" s="45"/>
       <c r="E70" s="45"/>
       <c r="F70" s="36" t="s">
@@ -7919,10 +7920,10 @@
       <c r="A71" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="B71" s="80" t="s">
+      <c r="B71" s="97" t="s">
         <v>129</v>
       </c>
-      <c r="C71" s="80"/>
+      <c r="C71" s="97"/>
       <c r="D71" s="47"/>
       <c r="E71" s="47"/>
       <c r="F71" s="36" t="s">
@@ -8001,10 +8002,10 @@
     </row>
     <row r="72" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="48"/>
-      <c r="B72" s="78" t="s">
+      <c r="B72" s="94" t="s">
         <v>130</v>
       </c>
-      <c r="C72" s="78"/>
+      <c r="C72" s="94"/>
       <c r="D72" s="45"/>
       <c r="E72" s="45"/>
       <c r="F72" s="36" t="s">
@@ -8083,14 +8084,14 @@
     </row>
     <row r="73" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="40"/>
-      <c r="B73" s="81" t="s">
+      <c r="B73" s="98" t="s">
         <v>131</v>
       </c>
-      <c r="C73" s="81"/>
-      <c r="D73" s="81">
+      <c r="C73" s="98"/>
+      <c r="D73" s="98">
         <v>35.200000000000003</v>
       </c>
-      <c r="E73" s="81"/>
+      <c r="E73" s="98"/>
       <c r="F73" s="36" t="s">
         <v>15</v>
       </c>
@@ -8168,10 +8169,10 @@
       <c r="A74" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="B74" s="78" t="s">
+      <c r="B74" s="94" t="s">
         <v>133</v>
       </c>
-      <c r="C74" s="78"/>
+      <c r="C74" s="94"/>
       <c r="D74" s="45"/>
       <c r="E74" s="45"/>
       <c r="F74" s="36" t="s">
@@ -8251,10 +8252,10 @@
       <c r="A75" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="B75" s="78" t="s">
+      <c r="B75" s="94" t="s">
         <v>135</v>
       </c>
-      <c r="C75" s="78"/>
+      <c r="C75" s="94"/>
       <c r="D75" s="45"/>
       <c r="E75" s="45"/>
       <c r="F75" s="36" t="s">
@@ -8334,10 +8335,10 @@
       <c r="A76" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="B76" s="78" t="s">
+      <c r="B76" s="94" t="s">
         <v>137</v>
       </c>
-      <c r="C76" s="78"/>
+      <c r="C76" s="94"/>
       <c r="D76" s="45"/>
       <c r="E76" s="45"/>
       <c r="F76" s="36" t="s">
@@ -8418,10 +8419,10 @@
       <c r="A77" s="35">
         <v>0</v>
       </c>
-      <c r="B77" s="78" t="s">
+      <c r="B77" s="94" t="s">
         <v>138</v>
       </c>
-      <c r="C77" s="78"/>
+      <c r="C77" s="94"/>
       <c r="D77" s="45"/>
       <c r="E77" s="45"/>
       <c r="F77" s="36" t="s">
@@ -8501,10 +8502,10 @@
       <c r="A78" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="B78" s="78" t="s">
+      <c r="B78" s="94" t="s">
         <v>140</v>
       </c>
-      <c r="C78" s="78"/>
+      <c r="C78" s="94"/>
       <c r="D78" s="45"/>
       <c r="E78" s="45"/>
       <c r="F78" s="36" t="s">
@@ -8585,10 +8586,10 @@
       <c r="A79" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="B79" s="78" t="s">
+      <c r="B79" s="94" t="s">
         <v>142</v>
       </c>
-      <c r="C79" s="78"/>
+      <c r="C79" s="94"/>
       <c r="D79" s="45"/>
       <c r="E79" s="45"/>
       <c r="F79" s="36" t="s">
@@ -8669,10 +8670,10 @@
       <c r="A80" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="B80" s="78" t="s">
-        <v>144</v>
-      </c>
-      <c r="C80" s="78"/>
+      <c r="B80" s="94" t="s">
+        <v>253</v>
+      </c>
+      <c r="C80" s="94"/>
       <c r="D80" s="45"/>
       <c r="E80" s="45"/>
       <c r="F80" s="36" t="s">
@@ -8750,12 +8751,12 @@
     </row>
     <row r="81" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="B81" s="94" t="s">
         <v>145</v>
       </c>
-      <c r="B81" s="78" t="s">
-        <v>146</v>
-      </c>
-      <c r="C81" s="78"/>
+      <c r="C81" s="94"/>
       <c r="D81" s="45"/>
       <c r="E81" s="45"/>
       <c r="F81" s="36" t="s">
@@ -8833,12 +8834,12 @@
     </row>
     <row r="82" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="35" t="s">
+        <v>146</v>
+      </c>
+      <c r="B82" s="94" t="s">
         <v>147</v>
       </c>
-      <c r="B82" s="78" t="s">
-        <v>148</v>
-      </c>
-      <c r="C82" s="78"/>
+      <c r="C82" s="94"/>
       <c r="D82" s="45"/>
       <c r="E82" s="45"/>
       <c r="F82" s="36" t="s">
@@ -8917,12 +8918,12 @@
     </row>
     <row r="83" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B83" s="94" t="s">
         <v>149</v>
       </c>
-      <c r="B83" s="78" t="s">
-        <v>150</v>
-      </c>
-      <c r="C83" s="78"/>
+      <c r="C83" s="94"/>
       <c r="D83" s="45"/>
       <c r="E83" s="45"/>
       <c r="F83" s="36" t="s">
@@ -9001,12 +9002,12 @@
     </row>
     <row r="84" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="B84" s="94" t="s">
         <v>151</v>
       </c>
-      <c r="B84" s="78" t="s">
-        <v>152</v>
-      </c>
-      <c r="C84" s="78"/>
+      <c r="C84" s="94"/>
       <c r="D84" s="45"/>
       <c r="E84" s="45"/>
       <c r="F84" s="36" t="s">
@@ -9085,12 +9086,12 @@
     </row>
     <row r="85" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="B85" s="94" t="s">
         <v>153</v>
       </c>
-      <c r="B85" s="78" t="s">
-        <v>154</v>
-      </c>
-      <c r="C85" s="78"/>
+      <c r="C85" s="94"/>
       <c r="D85" s="45"/>
       <c r="E85" s="45"/>
       <c r="F85" s="36" t="s">
@@ -9169,12 +9170,12 @@
     </row>
     <row r="86" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="B86" s="94" t="s">
         <v>155</v>
       </c>
-      <c r="B86" s="78" t="s">
-        <v>156</v>
-      </c>
-      <c r="C86" s="78"/>
+      <c r="C86" s="94"/>
       <c r="D86" s="45"/>
       <c r="E86" s="45"/>
       <c r="F86" s="36" t="s">
@@ -9253,12 +9254,12 @@
     </row>
     <row r="87" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="B87" s="94" t="s">
         <v>157</v>
       </c>
-      <c r="B87" s="78" t="s">
-        <v>158</v>
-      </c>
-      <c r="C87" s="78"/>
+      <c r="C87" s="94"/>
       <c r="D87" s="45"/>
       <c r="E87" s="45"/>
       <c r="F87" s="36" t="s">
@@ -9337,12 +9338,12 @@
     </row>
     <row r="88" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="B88" s="94" t="s">
         <v>159</v>
       </c>
-      <c r="B88" s="78" t="s">
-        <v>160</v>
-      </c>
-      <c r="C88" s="78"/>
+      <c r="C88" s="94"/>
       <c r="D88" s="45"/>
       <c r="E88" s="45"/>
       <c r="F88" s="36" t="s">
@@ -9420,12 +9421,12 @@
     </row>
     <row r="89" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="B89" s="94" t="s">
         <v>161</v>
       </c>
-      <c r="B89" s="78" t="s">
-        <v>162</v>
-      </c>
-      <c r="C89" s="78"/>
+      <c r="C89" s="94"/>
       <c r="D89" s="45"/>
       <c r="E89" s="45"/>
       <c r="F89" s="36" t="s">
@@ -9503,12 +9504,12 @@
     </row>
     <row r="90" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="35" t="s">
-        <v>163</v>
-      </c>
-      <c r="B90" s="78" t="s">
+        <v>162</v>
+      </c>
+      <c r="B90" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="78"/>
+      <c r="C90" s="94"/>
       <c r="D90" s="45"/>
       <c r="E90" s="45"/>
       <c r="F90" s="36" t="s">
@@ -9586,12 +9587,12 @@
     </row>
     <row r="91" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="35" t="s">
-        <v>164</v>
-      </c>
-      <c r="B91" s="78" t="s">
+        <v>163</v>
+      </c>
+      <c r="B91" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="78"/>
+      <c r="C91" s="94"/>
       <c r="D91" s="45"/>
       <c r="E91" s="45"/>
       <c r="F91" s="36" t="s">
@@ -9669,12 +9670,12 @@
     </row>
     <row r="92" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="35" t="s">
-        <v>165</v>
-      </c>
-      <c r="B92" s="78" t="s">
+        <v>164</v>
+      </c>
+      <c r="B92" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C92" s="78"/>
+      <c r="C92" s="94"/>
       <c r="D92" s="45"/>
       <c r="E92" s="45"/>
       <c r="F92" s="36" t="s">
@@ -9752,12 +9753,12 @@
     </row>
     <row r="93" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="B93" s="78" t="s">
+        <v>165</v>
+      </c>
+      <c r="B93" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C93" s="78"/>
+      <c r="C93" s="94"/>
       <c r="D93" s="45"/>
       <c r="E93" s="45"/>
       <c r="F93" s="36" t="s">
@@ -9835,12 +9836,12 @@
     </row>
     <row r="94" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="35" t="s">
-        <v>167</v>
-      </c>
-      <c r="B94" s="78" t="s">
+        <v>166</v>
+      </c>
+      <c r="B94" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C94" s="78"/>
+      <c r="C94" s="94"/>
       <c r="D94" s="45"/>
       <c r="E94" s="45"/>
       <c r="F94" s="36" t="s">
@@ -9918,12 +9919,12 @@
     </row>
     <row r="95" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="35" t="s">
-        <v>168</v>
-      </c>
-      <c r="B95" s="78" t="s">
+        <v>167</v>
+      </c>
+      <c r="B95" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C95" s="78"/>
+      <c r="C95" s="94"/>
       <c r="D95" s="45"/>
       <c r="E95" s="45"/>
       <c r="F95" s="36" t="s">
@@ -10001,12 +10002,12 @@
     </row>
     <row r="96" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="35" t="s">
-        <v>169</v>
-      </c>
-      <c r="B96" s="78" t="s">
+        <v>168</v>
+      </c>
+      <c r="B96" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C96" s="78"/>
+      <c r="C96" s="94"/>
       <c r="D96" s="45"/>
       <c r="E96" s="45"/>
       <c r="F96" s="36" t="s">
@@ -10084,12 +10085,12 @@
     </row>
     <row r="97" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="35" t="s">
-        <v>170</v>
-      </c>
-      <c r="B97" s="78" t="s">
+        <v>169</v>
+      </c>
+      <c r="B97" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C97" s="78"/>
+      <c r="C97" s="94"/>
       <c r="D97" s="45"/>
       <c r="E97" s="45"/>
       <c r="F97" s="36" t="s">
@@ -10167,12 +10168,12 @@
     </row>
     <row r="98" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="35" t="s">
-        <v>171</v>
-      </c>
-      <c r="B98" s="78" t="s">
+        <v>170</v>
+      </c>
+      <c r="B98" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C98" s="78"/>
+      <c r="C98" s="94"/>
       <c r="D98" s="45"/>
       <c r="E98" s="45"/>
       <c r="F98" s="36" t="s">
@@ -10250,12 +10251,12 @@
     </row>
     <row r="99" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="B99" s="94" t="s">
         <v>172</v>
       </c>
-      <c r="B99" s="78" t="s">
-        <v>173</v>
-      </c>
-      <c r="C99" s="78"/>
+      <c r="C99" s="94"/>
       <c r="D99" s="45"/>
       <c r="E99" s="45"/>
       <c r="F99" s="36" t="s">
@@ -10333,12 +10334,12 @@
     </row>
     <row r="100" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="35" t="s">
+        <v>173</v>
+      </c>
+      <c r="B100" s="94" t="s">
         <v>174</v>
       </c>
-      <c r="B100" s="78" t="s">
-        <v>175</v>
-      </c>
-      <c r="C100" s="78"/>
+      <c r="C100" s="94"/>
       <c r="D100" s="45"/>
       <c r="E100" s="45"/>
       <c r="F100" s="36" t="s">
@@ -10416,12 +10417,12 @@
     </row>
     <row r="101" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="35" t="s">
+        <v>175</v>
+      </c>
+      <c r="B101" s="99" t="s">
         <v>176</v>
       </c>
-      <c r="B101" s="79" t="s">
-        <v>177</v>
-      </c>
-      <c r="C101" s="79"/>
+      <c r="C101" s="99"/>
       <c r="D101" s="45"/>
       <c r="E101" s="45"/>
       <c r="F101" s="36" t="s">
@@ -10499,12 +10500,12 @@
     </row>
     <row r="102" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="35" t="s">
+        <v>177</v>
+      </c>
+      <c r="B102" s="94" t="s">
         <v>178</v>
       </c>
-      <c r="B102" s="78" t="s">
-        <v>179</v>
-      </c>
-      <c r="C102" s="78"/>
+      <c r="C102" s="94"/>
       <c r="D102" s="45"/>
       <c r="E102" s="45"/>
       <c r="F102" s="36" t="s">
@@ -10582,12 +10583,12 @@
     </row>
     <row r="103" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="35" t="s">
+        <v>179</v>
+      </c>
+      <c r="B103" s="94" t="s">
         <v>180</v>
       </c>
-      <c r="B103" s="78" t="s">
-        <v>181</v>
-      </c>
-      <c r="C103" s="78"/>
+      <c r="C103" s="94"/>
       <c r="D103" s="45"/>
       <c r="E103" s="45"/>
       <c r="F103" s="36" t="s">
@@ -10665,12 +10666,12 @@
     </row>
     <row r="104" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="35" t="s">
+        <v>181</v>
+      </c>
+      <c r="B104" s="94" t="s">
         <v>182</v>
       </c>
-      <c r="B104" s="78" t="s">
-        <v>183</v>
-      </c>
-      <c r="C104" s="78"/>
+      <c r="C104" s="94"/>
       <c r="D104" s="45"/>
       <c r="E104" s="45"/>
       <c r="F104" s="36" t="s">
@@ -10748,12 +10749,12 @@
     </row>
     <row r="105" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="B105" s="94" t="s">
         <v>184</v>
       </c>
-      <c r="B105" s="78" t="s">
-        <v>185</v>
-      </c>
-      <c r="C105" s="78"/>
+      <c r="C105" s="94"/>
       <c r="D105" s="45"/>
       <c r="E105" s="45"/>
       <c r="F105" s="36" t="s">
@@ -10831,12 +10832,12 @@
     </row>
     <row r="106" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="35" t="s">
+        <v>185</v>
+      </c>
+      <c r="B106" s="94" t="s">
         <v>186</v>
       </c>
-      <c r="B106" s="78" t="s">
-        <v>187</v>
-      </c>
-      <c r="C106" s="78"/>
+      <c r="C106" s="94"/>
       <c r="D106" s="45"/>
       <c r="E106" s="45"/>
       <c r="F106" s="36" t="s">
@@ -10914,12 +10915,12 @@
     </row>
     <row r="107" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="35" t="s">
+        <v>187</v>
+      </c>
+      <c r="B107" s="94" t="s">
         <v>188</v>
       </c>
-      <c r="B107" s="78" t="s">
-        <v>189</v>
-      </c>
-      <c r="C107" s="78"/>
+      <c r="C107" s="94"/>
       <c r="D107" s="45"/>
       <c r="E107" s="45"/>
       <c r="F107" s="36" t="s">
@@ -10997,12 +10998,12 @@
     </row>
     <row r="108" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="35" t="s">
+        <v>189</v>
+      </c>
+      <c r="B108" s="99" t="s">
         <v>190</v>
       </c>
-      <c r="B108" s="79" t="s">
-        <v>191</v>
-      </c>
-      <c r="C108" s="79"/>
+      <c r="C108" s="99"/>
       <c r="D108" s="45"/>
       <c r="E108" s="45"/>
       <c r="F108" s="36" t="s">
@@ -11080,12 +11081,12 @@
     </row>
     <row r="109" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="35" t="s">
-        <v>192</v>
-      </c>
-      <c r="B109" s="79" t="s">
         <v>191</v>
       </c>
-      <c r="C109" s="79"/>
+      <c r="B109" s="99" t="s">
+        <v>190</v>
+      </c>
+      <c r="C109" s="99"/>
       <c r="D109" s="45"/>
       <c r="E109" s="45"/>
       <c r="F109" s="36" t="s">
@@ -11163,12 +11164,12 @@
     </row>
     <row r="110" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="35" t="s">
-        <v>193</v>
-      </c>
-      <c r="B110" s="79" t="s">
-        <v>191</v>
-      </c>
-      <c r="C110" s="79"/>
+        <v>192</v>
+      </c>
+      <c r="B110" s="99" t="s">
+        <v>190</v>
+      </c>
+      <c r="C110" s="99"/>
       <c r="D110" s="45"/>
       <c r="E110" s="45"/>
       <c r="F110" s="36" t="s">
@@ -11246,12 +11247,12 @@
     </row>
     <row r="111" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="35" t="s">
-        <v>194</v>
-      </c>
-      <c r="B111" s="79" t="s">
-        <v>191</v>
-      </c>
-      <c r="C111" s="79"/>
+        <v>193</v>
+      </c>
+      <c r="B111" s="99" t="s">
+        <v>190</v>
+      </c>
+      <c r="C111" s="99"/>
       <c r="D111" s="45"/>
       <c r="E111" s="45"/>
       <c r="F111" s="36" t="s">
@@ -11329,12 +11330,12 @@
     </row>
     <row r="112" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="35" t="s">
-        <v>195</v>
-      </c>
-      <c r="B112" s="79" t="s">
-        <v>191</v>
-      </c>
-      <c r="C112" s="79"/>
+        <v>194</v>
+      </c>
+      <c r="B112" s="99" t="s">
+        <v>190</v>
+      </c>
+      <c r="C112" s="99"/>
       <c r="D112" s="45"/>
       <c r="E112" s="45"/>
       <c r="F112" s="36" t="s">
@@ -11412,12 +11413,12 @@
     </row>
     <row r="113" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="35" t="s">
-        <v>196</v>
-      </c>
-      <c r="B113" s="79" t="s">
-        <v>191</v>
-      </c>
-      <c r="C113" s="79"/>
+        <v>195</v>
+      </c>
+      <c r="B113" s="99" t="s">
+        <v>190</v>
+      </c>
+      <c r="C113" s="99"/>
       <c r="D113" s="45"/>
       <c r="E113" s="45"/>
       <c r="F113" s="36" t="s">
@@ -11495,12 +11496,12 @@
     </row>
     <row r="114" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="35" t="s">
-        <v>197</v>
-      </c>
-      <c r="B114" s="79" t="s">
-        <v>191</v>
-      </c>
-      <c r="C114" s="79"/>
+        <v>196</v>
+      </c>
+      <c r="B114" s="99" t="s">
+        <v>190</v>
+      </c>
+      <c r="C114" s="99"/>
       <c r="D114" s="45"/>
       <c r="E114" s="45"/>
       <c r="F114" s="36" t="s">
@@ -11578,12 +11579,12 @@
     </row>
     <row r="115" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="35" t="s">
+        <v>197</v>
+      </c>
+      <c r="B115" s="94" t="s">
         <v>198</v>
       </c>
-      <c r="B115" s="78" t="s">
-        <v>199</v>
-      </c>
-      <c r="C115" s="78"/>
+      <c r="C115" s="94"/>
       <c r="D115" s="45"/>
       <c r="E115" s="45"/>
       <c r="F115" s="36" t="s">
@@ -11661,12 +11662,12 @@
     </row>
     <row r="116" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="35" t="s">
+        <v>199</v>
+      </c>
+      <c r="B116" s="94" t="s">
         <v>200</v>
       </c>
-      <c r="B116" s="78" t="s">
-        <v>201</v>
-      </c>
-      <c r="C116" s="78"/>
+      <c r="C116" s="94"/>
       <c r="D116" s="45"/>
       <c r="E116" s="45"/>
       <c r="F116" s="36" t="s">
@@ -11744,12 +11745,12 @@
     </row>
     <row r="117" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="35" t="s">
+        <v>201</v>
+      </c>
+      <c r="B117" s="94" t="s">
         <v>202</v>
       </c>
-      <c r="B117" s="78" t="s">
-        <v>203</v>
-      </c>
-      <c r="C117" s="78"/>
+      <c r="C117" s="94"/>
       <c r="D117" s="45"/>
       <c r="E117" s="45"/>
       <c r="F117" s="36" t="s">
@@ -11827,12 +11828,12 @@
     </row>
     <row r="118" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="35" t="s">
+        <v>203</v>
+      </c>
+      <c r="B118" s="94" t="s">
         <v>204</v>
       </c>
-      <c r="B118" s="78" t="s">
-        <v>205</v>
-      </c>
-      <c r="C118" s="78"/>
+      <c r="C118" s="94"/>
       <c r="D118" s="45"/>
       <c r="E118" s="45"/>
       <c r="F118" s="36" t="s">
@@ -11910,12 +11911,12 @@
     </row>
     <row r="119" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="B119" s="94" t="s">
         <v>206</v>
       </c>
-      <c r="B119" s="78" t="s">
-        <v>207</v>
-      </c>
-      <c r="C119" s="78"/>
+      <c r="C119" s="94"/>
       <c r="D119" s="45"/>
       <c r="E119" s="45"/>
       <c r="F119" s="36" t="s">
@@ -11994,12 +11995,12 @@
     </row>
     <row r="120" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="35" t="s">
+        <v>207</v>
+      </c>
+      <c r="B120" s="94" t="s">
         <v>208</v>
       </c>
-      <c r="B120" s="78" t="s">
-        <v>209</v>
-      </c>
-      <c r="C120" s="78"/>
+      <c r="C120" s="94"/>
       <c r="D120" s="45"/>
       <c r="E120" s="45"/>
       <c r="F120" s="36" t="s">
@@ -12078,12 +12079,12 @@
     </row>
     <row r="121" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="35" t="s">
+        <v>209</v>
+      </c>
+      <c r="B121" s="94" t="s">
         <v>210</v>
       </c>
-      <c r="B121" s="78" t="s">
-        <v>211</v>
-      </c>
-      <c r="C121" s="78"/>
+      <c r="C121" s="94"/>
       <c r="D121" s="45"/>
       <c r="E121" s="45"/>
       <c r="F121" s="36" t="s">
@@ -12161,12 +12162,12 @@
     </row>
     <row r="122" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="35" t="s">
+        <v>211</v>
+      </c>
+      <c r="B122" s="94" t="s">
         <v>212</v>
       </c>
-      <c r="B122" s="78" t="s">
-        <v>213</v>
-      </c>
-      <c r="C122" s="78"/>
+      <c r="C122" s="94"/>
       <c r="D122" s="45"/>
       <c r="E122" s="45"/>
       <c r="F122" s="36" t="s">
@@ -12244,12 +12245,12 @@
     </row>
     <row r="123" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="35" t="s">
+        <v>213</v>
+      </c>
+      <c r="B123" s="94" t="s">
         <v>214</v>
       </c>
-      <c r="B123" s="78" t="s">
-        <v>215</v>
-      </c>
-      <c r="C123" s="78"/>
+      <c r="C123" s="94"/>
       <c r="D123" s="45"/>
       <c r="E123" s="45"/>
       <c r="F123" s="36" t="s">
@@ -12327,12 +12328,12 @@
     </row>
     <row r="124" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="B124" s="94" t="s">
         <v>216</v>
       </c>
-      <c r="B124" s="78" t="s">
-        <v>217</v>
-      </c>
-      <c r="C124" s="78"/>
+      <c r="C124" s="94"/>
       <c r="D124" s="45"/>
       <c r="E124" s="45"/>
       <c r="F124" s="36" t="s">
@@ -12410,12 +12411,12 @@
     </row>
     <row r="125" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="B125" s="94" t="s">
         <v>218</v>
       </c>
-      <c r="B125" s="78" t="s">
-        <v>219</v>
-      </c>
-      <c r="C125" s="78"/>
+      <c r="C125" s="94"/>
       <c r="D125" s="45"/>
       <c r="E125" s="45"/>
       <c r="F125" s="36" t="s">
@@ -12493,12 +12494,12 @@
     </row>
     <row r="126" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="35" t="s">
+        <v>219</v>
+      </c>
+      <c r="B126" s="94" t="s">
         <v>220</v>
       </c>
-      <c r="B126" s="78" t="s">
-        <v>221</v>
-      </c>
-      <c r="C126" s="78"/>
+      <c r="C126" s="94"/>
       <c r="D126" s="45"/>
       <c r="E126" s="45"/>
       <c r="F126" s="36" t="s">
@@ -12576,12 +12577,12 @@
     </row>
     <row r="127" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="35" t="s">
+        <v>221</v>
+      </c>
+      <c r="B127" s="94" t="s">
         <v>222</v>
       </c>
-      <c r="B127" s="78" t="s">
-        <v>223</v>
-      </c>
-      <c r="C127" s="78"/>
+      <c r="C127" s="94"/>
       <c r="D127" s="45"/>
       <c r="E127" s="45"/>
       <c r="F127" s="36" t="s">
@@ -12659,12 +12660,12 @@
     </row>
     <row r="128" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="35" t="s">
+        <v>223</v>
+      </c>
+      <c r="B128" s="94" t="s">
         <v>224</v>
       </c>
-      <c r="B128" s="78" t="s">
-        <v>225</v>
-      </c>
-      <c r="C128" s="78"/>
+      <c r="C128" s="94"/>
       <c r="D128" s="45"/>
       <c r="E128" s="45"/>
       <c r="F128" s="36" t="s">
@@ -12742,12 +12743,12 @@
     </row>
     <row r="129" spans="1:255" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="35" t="s">
+        <v>225</v>
+      </c>
+      <c r="B129" s="94" t="s">
         <v>226</v>
       </c>
-      <c r="B129" s="78" t="s">
-        <v>227</v>
-      </c>
-      <c r="C129" s="78"/>
+      <c r="C129" s="94"/>
       <c r="D129" s="45"/>
       <c r="E129" s="45"/>
       <c r="F129" s="36" t="s">
@@ -12825,12 +12826,12 @@
     </row>
     <row r="130" spans="1:255" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="35" t="s">
+        <v>227</v>
+      </c>
+      <c r="B130" s="94" t="s">
         <v>228</v>
       </c>
-      <c r="B130" s="78" t="s">
-        <v>229</v>
-      </c>
-      <c r="C130" s="78"/>
+      <c r="C130" s="94"/>
       <c r="D130" s="45"/>
       <c r="E130" s="45"/>
       <c r="F130" s="36" t="s">
@@ -12908,12 +12909,12 @@
     </row>
     <row r="131" spans="1:255" s="51" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="35" t="s">
+        <v>229</v>
+      </c>
+      <c r="B131" s="91" t="s">
         <v>230</v>
       </c>
-      <c r="B131" s="77" t="s">
-        <v>231</v>
-      </c>
-      <c r="C131" s="77"/>
+      <c r="C131" s="91"/>
       <c r="D131" s="36"/>
       <c r="E131" s="36"/>
       <c r="F131" s="36" t="s">
@@ -13217,14 +13218,14 @@
     </row>
     <row r="132" spans="1:255" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="52" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B132" s="53"/>
       <c r="C132" s="54"/>
       <c r="D132" s="55"/>
       <c r="E132" s="49"/>
       <c r="F132" s="56" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G132" s="49"/>
       <c r="H132" s="57"/>
@@ -13250,7 +13251,7 @@
     </row>
     <row r="133" spans="1:255" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="63" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B133" s="64"/>
       <c r="C133" s="65"/>
@@ -13277,7 +13278,7 @@
     </row>
     <row r="134" spans="1:255" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="76" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B134" s="67"/>
       <c r="C134" s="2"/>
@@ -13304,7 +13305,7 @@
     </row>
     <row r="135" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="76" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B135" s="67"/>
       <c r="C135" s="2"/>
@@ -13331,7 +13332,7 @@
     </row>
     <row r="136" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="63" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B136" s="67"/>
       <c r="C136" s="2"/>
@@ -13358,7 +13359,7 @@
     </row>
     <row r="137" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="63" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B137" s="67"/>
       <c r="C137" s="2"/>
@@ -13385,7 +13386,7 @@
     </row>
     <row r="138" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="63" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B138" s="67"/>
       <c r="C138" s="2"/>
@@ -13412,7 +13413,7 @@
     </row>
     <row r="139" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="63" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B139" s="67"/>
       <c r="C139" s="2"/>
@@ -13439,7 +13440,7 @@
     </row>
     <row r="140" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="63" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B140" s="67"/>
       <c r="C140" s="2"/>
@@ -13466,7 +13467,7 @@
     </row>
     <row r="141" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="63" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B141" s="67"/>
       <c r="C141" s="2"/>
@@ -13493,7 +13494,7 @@
     </row>
     <row r="142" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="63" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B142" s="67"/>
       <c r="C142" s="2"/>
@@ -13520,7 +13521,7 @@
     </row>
     <row r="143" spans="1:255" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="76" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B143" s="64"/>
       <c r="C143" s="65"/>
@@ -13542,7 +13543,7 @@
     </row>
     <row r="144" spans="1:255" s="61" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="76" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B144" s="64"/>
       <c r="C144" s="65"/>
@@ -13569,7 +13570,7 @@
     </row>
     <row r="145" spans="1:46" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="76" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B145" s="71"/>
       <c r="C145" s="72"/>
@@ -13596,7 +13597,7 @@
     </row>
     <row r="146" spans="1:46" s="61" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="76" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B146" s="64"/>
       <c r="C146" s="65"/>
@@ -13623,7 +13624,7 @@
     </row>
     <row r="147" spans="1:46" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="76" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B147" s="64"/>
       <c r="C147" s="65"/>
@@ -13650,7 +13651,7 @@
     </row>
     <row r="148" spans="1:46" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="76" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B148" s="64"/>
       <c r="C148" s="65"/>
@@ -14179,6 +14180,133 @@
     </row>
   </sheetData>
   <mergeCells count="141">
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A2:U2"/>
     <mergeCell ref="J5:K5"/>
@@ -14193,133 +14321,6 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:S7"/>
     <mergeCell ref="T7:U7"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="B130:C130"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Update dailyreport template remark
1. update dailyreport template remark
2. update watchlist garlic low price action
</commit_message>
<xml_diff>
--- a/src/apps/dailytrans/reports/template.xlsx
+++ b/src/apps/dailytrans/reports/template.xlsx
@@ -863,9 +863,6 @@
   </si>
   <si>
     <t>註：</t>
-  </si>
-  <si>
-    <t>表該產品最近連續一週價格低於監控價格；</t>
   </si>
   <si>
     <r>
@@ -1459,6 +1456,10 @@
   <si>
     <t>鳳梨釋迦
 (產地)</t>
+    <phoneticPr fontId="26" type="noConversion"/>
+  </si>
+  <si>
+    <t>表該產品最近連續一週價格低或高於監控價格；</t>
     <phoneticPr fontId="26" type="noConversion"/>
   </si>
 </sst>
@@ -2029,6 +2030,36 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="180" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="21" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2067,36 +2098,6 @@
     </xf>
     <xf numFmtId="179" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="21" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2474,8 +2475,8 @@
   <dimension ref="A1:AMJ256"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B91" sqref="B91:C91"/>
+      <pane ySplit="8" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M132" sqref="M132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -2509,35 +2510,35 @@
       <c r="F1" s="8"/>
       <c r="G1" s="9"/>
       <c r="H1" s="10"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
       <c r="M1" s="11"/>
       <c r="N1" s="11"/>
     </row>
     <row r="2" spans="1:30" s="12" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
-      <c r="N2" s="78"/>
-      <c r="O2" s="78"/>
-      <c r="P2" s="78"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="78"/>
-      <c r="S2" s="78"/>
-      <c r="T2" s="78"/>
-      <c r="U2" s="78"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="88"/>
+      <c r="I2" s="88"/>
+      <c r="J2" s="88"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
+      <c r="Q2" s="88"/>
+      <c r="R2" s="88"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="88"/>
     </row>
     <row r="3" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="13"/>
@@ -2586,8 +2587,8 @@
       <c r="G5" s="20"/>
       <c r="H5" s="21"/>
       <c r="I5" s="22"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
       <c r="L5" s="21"/>
       <c r="M5" s="23"/>
       <c r="N5" s="23"/>
@@ -2596,41 +2597,41 @@
       <c r="S5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="T5" s="80" t="s">
+      <c r="T5" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="U5" s="80"/>
+      <c r="U5" s="90"/>
     </row>
     <row r="6" spans="1:30" s="12" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="82"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="84" t="s">
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="85" t="s">
+      <c r="G6" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="81" t="s">
+      <c r="H6" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="81"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="81"/>
-      <c r="L6" s="81"/>
-      <c r="M6" s="81"/>
-      <c r="N6" s="81"/>
-      <c r="O6" s="81"/>
-      <c r="P6" s="81"/>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="81"/>
-      <c r="S6" s="81"/>
-      <c r="T6" s="81"/>
-      <c r="U6" s="81"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
+      <c r="O6" s="91"/>
+      <c r="P6" s="91"/>
+      <c r="Q6" s="91"/>
+      <c r="R6" s="91"/>
+      <c r="S6" s="91"/>
+      <c r="T6" s="91"/>
+      <c r="U6" s="91"/>
       <c r="V6" s="1"/>
       <c r="W6" s="28"/>
       <c r="X6" s="28"/>
@@ -2642,36 +2643,36 @@
       <c r="AD6" s="28"/>
     </row>
     <row r="7" spans="1:30" s="12" customFormat="1" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="81"/>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="85"/>
-      <c r="H7" s="86" t="s">
+      <c r="A7" s="91"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="91"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="96" t="s">
         <v>7</v>
       </c>
       <c r="I7" s="29"/>
       <c r="J7" s="29"/>
       <c r="K7" s="29"/>
-      <c r="L7" s="87" t="s">
-        <v>246</v>
-      </c>
-      <c r="M7" s="88" t="s">
+      <c r="L7" s="97" t="s">
+        <v>245</v>
+      </c>
+      <c r="M7" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="88"/>
-      <c r="O7" s="88"/>
-      <c r="P7" s="88"/>
-      <c r="Q7" s="88"/>
-      <c r="R7" s="88"/>
-      <c r="S7" s="88"/>
-      <c r="T7" s="89" t="s">
+      <c r="N7" s="98"/>
+      <c r="O7" s="98"/>
+      <c r="P7" s="98"/>
+      <c r="Q7" s="98"/>
+      <c r="R7" s="98"/>
+      <c r="S7" s="98"/>
+      <c r="T7" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="U7" s="89"/>
-      <c r="V7" s="90"/>
+      <c r="U7" s="99"/>
+      <c r="V7" s="84"/>
       <c r="W7" s="30"/>
       <c r="X7" s="30"/>
       <c r="Y7" s="30"/>
@@ -2682,14 +2683,14 @@
       <c r="AD7" s="30"/>
     </row>
     <row r="8" spans="1:30" s="12" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="81"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="82"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="86"/>
+      <c r="A8" s="91"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="91"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="95"/>
+      <c r="H8" s="96"/>
       <c r="I8" s="31" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -2702,9 +2703,9 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="L8" s="87"/>
+      <c r="L8" s="97"/>
       <c r="M8" s="32" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N8" s="32" t="s">
         <v>10</v>
@@ -2728,9 +2729,9 @@
         <v>11</v>
       </c>
       <c r="U8" s="33" t="s">
-        <v>248</v>
-      </c>
-      <c r="V8" s="90"/>
+        <v>247</v>
+      </c>
+      <c r="V8" s="84"/>
       <c r="W8" s="34" t="s">
         <v>12</v>
       </c>
@@ -2760,13 +2761,13 @@
       <c r="A9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="91" t="s">
+      <c r="B9" s="77" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="91"/>
-      <c r="D9" s="92"/>
-      <c r="E9" s="92"/>
-      <c r="F9" s="93" t="s">
+      <c r="C9" s="77"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="86" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="37" t="s">
@@ -2843,13 +2844,13 @@
       <c r="A10" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="91"/>
-      <c r="D10" s="92"/>
-      <c r="E10" s="92"/>
-      <c r="F10" s="92"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
       <c r="G10" s="37" t="s">
         <v>15</v>
       </c>
@@ -2924,10 +2925,10 @@
       <c r="A11" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="91"/>
+      <c r="C11" s="77"/>
       <c r="D11" s="36" t="s">
         <v>15</v>
       </c>
@@ -3011,10 +3012,10 @@
       <c r="A12" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="91" t="s">
+      <c r="B12" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="91"/>
+      <c r="C12" s="77"/>
       <c r="D12" s="36" t="s">
         <v>15</v>
       </c>
@@ -3098,10 +3099,10 @@
       <c r="A13" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="91" t="s">
+      <c r="B13" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="91"/>
+      <c r="C13" s="77"/>
       <c r="D13" s="36" t="s">
         <v>15</v>
       </c>
@@ -3185,10 +3186,10 @@
       <c r="A14" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="94" t="s">
+      <c r="B14" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="94"/>
+      <c r="C14" s="78"/>
       <c r="D14" s="43"/>
       <c r="E14" s="43"/>
       <c r="F14" s="36" t="s">
@@ -3269,10 +3270,10 @@
       <c r="A15" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="94" t="s">
+      <c r="B15" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="94"/>
+      <c r="C15" s="78"/>
       <c r="D15" s="43"/>
       <c r="E15" s="43"/>
       <c r="F15" s="36" t="s">
@@ -3352,10 +3353,10 @@
       <c r="A16" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="94" t="s">
+      <c r="B16" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="94"/>
+      <c r="C16" s="78"/>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
       <c r="F16" s="36" t="s">
@@ -3435,10 +3436,10 @@
       <c r="A17" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="94" t="s">
+      <c r="B17" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="94"/>
+      <c r="C17" s="78"/>
       <c r="D17" s="43"/>
       <c r="E17" s="43"/>
       <c r="F17" s="36" t="s">
@@ -3518,10 +3519,10 @@
       <c r="A18" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="95" t="s">
+      <c r="B18" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="95"/>
+      <c r="C18" s="83"/>
       <c r="D18" s="43"/>
       <c r="E18" s="43"/>
       <c r="F18" s="36" t="s">
@@ -3601,10 +3602,10 @@
       <c r="A19" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="94"/>
+      <c r="C19" s="78"/>
       <c r="D19" s="43"/>
       <c r="E19" s="43"/>
       <c r="F19" s="36" t="s">
@@ -3684,10 +3685,10 @@
       <c r="A20" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="94" t="s">
+      <c r="B20" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="94"/>
+      <c r="C20" s="78"/>
       <c r="D20" s="43"/>
       <c r="E20" s="43"/>
       <c r="F20" s="36" t="s">
@@ -3767,10 +3768,10 @@
       <c r="A21" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="94" t="s">
+      <c r="B21" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="94"/>
+      <c r="C21" s="78"/>
       <c r="D21" s="43"/>
       <c r="E21" s="43"/>
       <c r="F21" s="36" t="s">
@@ -3850,10 +3851,10 @@
       <c r="A22" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="94" t="s">
+      <c r="B22" s="78" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="94"/>
+      <c r="C22" s="78"/>
       <c r="D22" s="43"/>
       <c r="E22" s="43"/>
       <c r="F22" s="36" t="s">
@@ -3933,10 +3934,10 @@
       <c r="A23" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="94" t="s">
+      <c r="B23" s="78" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="94"/>
+      <c r="C23" s="78"/>
       <c r="D23" s="43"/>
       <c r="E23" s="43"/>
       <c r="F23" s="36" t="s">
@@ -4016,10 +4017,10 @@
       <c r="A24" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="94" t="s">
+      <c r="B24" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="94"/>
+      <c r="C24" s="78"/>
       <c r="D24" s="43"/>
       <c r="E24" s="43"/>
       <c r="F24" s="36" t="s">
@@ -4099,10 +4100,10 @@
       <c r="A25" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="95" t="s">
+      <c r="B25" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="95"/>
+      <c r="C25" s="83"/>
       <c r="D25" s="43"/>
       <c r="E25" s="43"/>
       <c r="F25" s="36" t="s">
@@ -4182,10 +4183,10 @@
       <c r="A26" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="94" t="s">
+      <c r="B26" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="94"/>
+      <c r="C26" s="78"/>
       <c r="D26" s="43"/>
       <c r="E26" s="43"/>
       <c r="F26" s="36" t="s">
@@ -4265,10 +4266,10 @@
       <c r="A27" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="94" t="s">
+      <c r="B27" s="78" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="94"/>
+      <c r="C27" s="78"/>
       <c r="D27" s="43"/>
       <c r="E27" s="43"/>
       <c r="F27" s="36" t="s">
@@ -4348,10 +4349,10 @@
       <c r="A28" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="94" t="s">
+      <c r="B28" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="94"/>
+      <c r="C28" s="78"/>
       <c r="D28" s="43"/>
       <c r="E28" s="43"/>
       <c r="F28" s="36" t="s">
@@ -4431,10 +4432,10 @@
       <c r="A29" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="95" t="s">
+      <c r="B29" s="83" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="95"/>
+      <c r="C29" s="83"/>
       <c r="D29" s="43"/>
       <c r="E29" s="43"/>
       <c r="F29" s="36" t="s">
@@ -4515,10 +4516,10 @@
       <c r="A30" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="95" t="s">
+      <c r="B30" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="95"/>
+      <c r="C30" s="83"/>
       <c r="D30" s="43"/>
       <c r="E30" s="43"/>
       <c r="F30" s="36" t="s">
@@ -4599,10 +4600,10 @@
       <c r="A31" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="94" t="s">
+      <c r="B31" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="94"/>
+      <c r="C31" s="78"/>
       <c r="D31" s="43"/>
       <c r="E31" s="43"/>
       <c r="F31" s="36" t="s">
@@ -4682,10 +4683,10 @@
       <c r="A32" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="94" t="s">
+      <c r="B32" s="78" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="94"/>
+      <c r="C32" s="78"/>
       <c r="D32" s="43"/>
       <c r="E32" s="43"/>
       <c r="F32" s="36" t="s">
@@ -4765,10 +4766,10 @@
       <c r="A33" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="94" t="s">
+      <c r="B33" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="94"/>
+      <c r="C33" s="78"/>
       <c r="D33" s="45"/>
       <c r="E33" s="45"/>
       <c r="F33" s="36" t="s">
@@ -4849,10 +4850,10 @@
       <c r="A34" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="94" t="s">
+      <c r="B34" s="78" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="94"/>
+      <c r="C34" s="78"/>
       <c r="D34" s="45"/>
       <c r="E34" s="45"/>
       <c r="F34" s="36" t="s">
@@ -4932,10 +4933,10 @@
       <c r="A35" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="94" t="s">
+      <c r="B35" s="78" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="94"/>
+      <c r="C35" s="78"/>
       <c r="D35" s="45"/>
       <c r="E35" s="45"/>
       <c r="F35" s="36" t="s">
@@ -5015,10 +5016,10 @@
       <c r="A36" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="94" t="s">
+      <c r="B36" s="78" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="94"/>
+      <c r="C36" s="78"/>
       <c r="D36" s="45"/>
       <c r="E36" s="45"/>
       <c r="F36" s="36" t="s">
@@ -5098,10 +5099,10 @@
       <c r="A37" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="94" t="s">
+      <c r="B37" s="78" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="94"/>
+      <c r="C37" s="78"/>
       <c r="D37" s="45"/>
       <c r="E37" s="45"/>
       <c r="F37" s="36" t="s">
@@ -5181,10 +5182,10 @@
       <c r="A38" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="94" t="s">
+      <c r="B38" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="94"/>
+      <c r="C38" s="78"/>
       <c r="D38" s="45"/>
       <c r="E38" s="45"/>
       <c r="F38" s="36" t="s">
@@ -5264,10 +5265,10 @@
       <c r="A39" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="94" t="s">
+      <c r="B39" s="78" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="94"/>
+      <c r="C39" s="78"/>
       <c r="D39" s="45"/>
       <c r="E39" s="45"/>
       <c r="F39" s="36" t="s">
@@ -5347,10 +5348,10 @@
       <c r="A40" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="94" t="s">
+      <c r="B40" s="78" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="94"/>
+      <c r="C40" s="78"/>
       <c r="D40" s="45"/>
       <c r="E40" s="45"/>
       <c r="F40" s="36" t="s">
@@ -5430,10 +5431,10 @@
       <c r="A41" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="94" t="s">
+      <c r="B41" s="78" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="94"/>
+      <c r="C41" s="78"/>
       <c r="D41" s="45"/>
       <c r="E41" s="45"/>
       <c r="F41" s="36" t="s">
@@ -5513,10 +5514,10 @@
       <c r="A42" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="94" t="s">
+      <c r="B42" s="78" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="94"/>
+      <c r="C42" s="78"/>
       <c r="D42" s="45"/>
       <c r="E42" s="45"/>
       <c r="F42" s="36" t="s">
@@ -5597,10 +5598,10 @@
       <c r="A43" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="96" t="s">
+      <c r="B43" s="82" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="96"/>
+      <c r="C43" s="82"/>
       <c r="D43" s="45"/>
       <c r="E43" s="45"/>
       <c r="F43" s="36" t="s">
@@ -5680,10 +5681,10 @@
       <c r="A44" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="96" t="s">
+      <c r="B44" s="82" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="96"/>
+      <c r="C44" s="82"/>
       <c r="D44" s="45"/>
       <c r="E44" s="45"/>
       <c r="F44" s="36" t="s">
@@ -5763,10 +5764,10 @@
       <c r="A45" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="94" t="s">
+      <c r="B45" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="94"/>
+      <c r="C45" s="78"/>
       <c r="D45" s="45"/>
       <c r="E45" s="45"/>
       <c r="F45" s="36" t="s">
@@ -5846,10 +5847,10 @@
       <c r="A46" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="94" t="s">
+      <c r="B46" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="94"/>
+      <c r="C46" s="78"/>
       <c r="D46" s="45"/>
       <c r="E46" s="45"/>
       <c r="F46" s="36" t="s">
@@ -5929,10 +5930,10 @@
       <c r="A47" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="94" t="s">
+      <c r="B47" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C47" s="94"/>
+      <c r="C47" s="78"/>
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
       <c r="F47" s="36" t="s">
@@ -6012,10 +6013,10 @@
       <c r="A48" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="94" t="s">
+      <c r="B48" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="94"/>
+      <c r="C48" s="78"/>
       <c r="D48" s="45"/>
       <c r="E48" s="45"/>
       <c r="F48" s="36" t="s">
@@ -6095,10 +6096,10 @@
       <c r="A49" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="94" t="s">
+      <c r="B49" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C49" s="94"/>
+      <c r="C49" s="78"/>
       <c r="D49" s="45"/>
       <c r="E49" s="45"/>
       <c r="F49" s="36" t="s">
@@ -6178,10 +6179,10 @@
       <c r="A50" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="94" t="s">
+      <c r="B50" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C50" s="94"/>
+      <c r="C50" s="78"/>
       <c r="D50" s="45"/>
       <c r="E50" s="45"/>
       <c r="F50" s="36" t="s">
@@ -6261,10 +6262,10 @@
       <c r="A51" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="94" t="s">
+      <c r="B51" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C51" s="94"/>
+      <c r="C51" s="78"/>
       <c r="D51" s="45"/>
       <c r="E51" s="45"/>
       <c r="F51" s="36" t="s">
@@ -6344,10 +6345,10 @@
       <c r="A52" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="94" t="s">
+      <c r="B52" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="94"/>
+      <c r="C52" s="78"/>
       <c r="D52" s="45"/>
       <c r="E52" s="45"/>
       <c r="F52" s="36" t="s">
@@ -6427,10 +6428,10 @@
       <c r="A53" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="94" t="s">
+      <c r="B53" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="94"/>
+      <c r="C53" s="78"/>
       <c r="D53" s="45"/>
       <c r="E53" s="45"/>
       <c r="F53" s="36" t="s">
@@ -6510,10 +6511,10 @@
       <c r="A54" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="B54" s="94" t="s">
+      <c r="B54" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="94"/>
+      <c r="C54" s="78"/>
       <c r="D54" s="45"/>
       <c r="E54" s="45"/>
       <c r="F54" s="36" t="s">
@@ -6593,10 +6594,10 @@
       <c r="A55" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="B55" s="94" t="s">
+      <c r="B55" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C55" s="94"/>
+      <c r="C55" s="78"/>
       <c r="D55" s="45"/>
       <c r="E55" s="45"/>
       <c r="F55" s="36" t="s">
@@ -6676,10 +6677,10 @@
       <c r="A56" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="B56" s="94" t="s">
+      <c r="B56" s="78" t="s">
         <v>100</v>
       </c>
-      <c r="C56" s="94"/>
+      <c r="C56" s="78"/>
       <c r="D56" s="45"/>
       <c r="E56" s="45"/>
       <c r="F56" s="36" t="s">
@@ -6759,10 +6760,10 @@
       <c r="A57" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="B57" s="94" t="s">
+      <c r="B57" s="78" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="94"/>
+      <c r="C57" s="78"/>
       <c r="D57" s="45"/>
       <c r="E57" s="45"/>
       <c r="F57" s="36" t="s">
@@ -6842,10 +6843,10 @@
       <c r="A58" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="B58" s="94" t="s">
+      <c r="B58" s="78" t="s">
         <v>104</v>
       </c>
-      <c r="C58" s="94"/>
+      <c r="C58" s="78"/>
       <c r="D58" s="45"/>
       <c r="E58" s="45"/>
       <c r="F58" s="36" t="s">
@@ -6925,10 +6926,10 @@
       <c r="A59" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="B59" s="94" t="s">
+      <c r="B59" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="C59" s="94"/>
+      <c r="C59" s="78"/>
       <c r="D59" s="45"/>
       <c r="E59" s="45"/>
       <c r="F59" s="36" t="s">
@@ -7008,10 +7009,10 @@
       <c r="A60" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="B60" s="94" t="s">
+      <c r="B60" s="78" t="s">
         <v>108</v>
       </c>
-      <c r="C60" s="94"/>
+      <c r="C60" s="78"/>
       <c r="D60" s="45"/>
       <c r="E60" s="45"/>
       <c r="F60" s="36" t="s">
@@ -7091,10 +7092,10 @@
       <c r="A61" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="B61" s="94" t="s">
+      <c r="B61" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="C61" s="94"/>
+      <c r="C61" s="78"/>
       <c r="D61" s="45"/>
       <c r="E61" s="45"/>
       <c r="F61" s="36" t="s">
@@ -7174,10 +7175,10 @@
       <c r="A62" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="B62" s="94" t="s">
+      <c r="B62" s="78" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="94"/>
+      <c r="C62" s="78"/>
       <c r="D62" s="45"/>
       <c r="E62" s="45"/>
       <c r="F62" s="36" t="s">
@@ -7258,10 +7259,10 @@
       <c r="A63" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="B63" s="94" t="s">
-        <v>252</v>
-      </c>
-      <c r="C63" s="94"/>
+      <c r="B63" s="78" t="s">
+        <v>251</v>
+      </c>
+      <c r="C63" s="78"/>
       <c r="D63" s="45"/>
       <c r="E63" s="45"/>
       <c r="F63" s="36" t="s">
@@ -7341,10 +7342,10 @@
       <c r="A64" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="B64" s="94" t="s">
+      <c r="B64" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="C64" s="94"/>
+      <c r="C64" s="78"/>
       <c r="D64" s="45"/>
       <c r="E64" s="45"/>
       <c r="F64" s="36" t="s">
@@ -7425,10 +7426,10 @@
       <c r="A65" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="B65" s="94" t="s">
+      <c r="B65" s="78" t="s">
         <v>117</v>
       </c>
-      <c r="C65" s="94"/>
+      <c r="C65" s="78"/>
       <c r="D65" s="45"/>
       <c r="E65" s="45"/>
       <c r="F65" s="36" t="s">
@@ -7508,10 +7509,10 @@
       <c r="A66" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="94" t="s">
+      <c r="B66" s="78" t="s">
         <v>119</v>
       </c>
-      <c r="C66" s="94"/>
+      <c r="C66" s="78"/>
       <c r="D66" s="45"/>
       <c r="E66" s="45"/>
       <c r="F66" s="36" t="s">
@@ -7592,10 +7593,10 @@
       <c r="A67" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="B67" s="94" t="s">
+      <c r="B67" s="78" t="s">
         <v>121</v>
       </c>
-      <c r="C67" s="94"/>
+      <c r="C67" s="78"/>
       <c r="D67" s="45"/>
       <c r="E67" s="45"/>
       <c r="F67" s="36" t="s">
@@ -7675,10 +7676,10 @@
       <c r="A68" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B68" s="94" t="s">
+      <c r="B68" s="78" t="s">
         <v>123</v>
       </c>
-      <c r="C68" s="94"/>
+      <c r="C68" s="78"/>
       <c r="D68" s="45"/>
       <c r="E68" s="45"/>
       <c r="F68" s="36" t="s">
@@ -7758,10 +7759,10 @@
       <c r="A69" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="B69" s="94" t="s">
+      <c r="B69" s="78" t="s">
         <v>125</v>
       </c>
-      <c r="C69" s="94"/>
+      <c r="C69" s="78"/>
       <c r="D69" s="45"/>
       <c r="E69" s="45"/>
       <c r="F69" s="36" t="s">
@@ -7842,10 +7843,10 @@
       <c r="A70" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="B70" s="94" t="s">
+      <c r="B70" s="78" t="s">
         <v>127</v>
       </c>
-      <c r="C70" s="94"/>
+      <c r="C70" s="78"/>
       <c r="D70" s="45"/>
       <c r="E70" s="45"/>
       <c r="F70" s="36" t="s">
@@ -7925,10 +7926,10 @@
       <c r="A71" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="B71" s="97" t="s">
+      <c r="B71" s="80" t="s">
         <v>129</v>
       </c>
-      <c r="C71" s="97"/>
+      <c r="C71" s="80"/>
       <c r="D71" s="47"/>
       <c r="E71" s="47"/>
       <c r="F71" s="36" t="s">
@@ -8007,10 +8008,10 @@
     </row>
     <row r="72" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="48"/>
-      <c r="B72" s="94" t="s">
+      <c r="B72" s="78" t="s">
         <v>130</v>
       </c>
-      <c r="C72" s="94"/>
+      <c r="C72" s="78"/>
       <c r="D72" s="45"/>
       <c r="E72" s="45"/>
       <c r="F72" s="36" t="s">
@@ -8089,14 +8090,14 @@
     </row>
     <row r="73" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="40"/>
-      <c r="B73" s="98" t="s">
+      <c r="B73" s="81" t="s">
         <v>131</v>
       </c>
-      <c r="C73" s="98"/>
-      <c r="D73" s="98">
+      <c r="C73" s="81"/>
+      <c r="D73" s="81">
         <v>35.200000000000003</v>
       </c>
-      <c r="E73" s="98"/>
+      <c r="E73" s="81"/>
       <c r="F73" s="36" t="s">
         <v>15</v>
       </c>
@@ -8174,10 +8175,10 @@
       <c r="A74" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="B74" s="94" t="s">
+      <c r="B74" s="78" t="s">
         <v>133</v>
       </c>
-      <c r="C74" s="94"/>
+      <c r="C74" s="78"/>
       <c r="D74" s="45"/>
       <c r="E74" s="45"/>
       <c r="F74" s="36" t="s">
@@ -8257,10 +8258,10 @@
       <c r="A75" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="B75" s="94" t="s">
+      <c r="B75" s="78" t="s">
         <v>135</v>
       </c>
-      <c r="C75" s="94"/>
+      <c r="C75" s="78"/>
       <c r="D75" s="45"/>
       <c r="E75" s="45"/>
       <c r="F75" s="36" t="s">
@@ -8340,10 +8341,10 @@
       <c r="A76" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="B76" s="94" t="s">
+      <c r="B76" s="78" t="s">
         <v>137</v>
       </c>
-      <c r="C76" s="94"/>
+      <c r="C76" s="78"/>
       <c r="D76" s="45"/>
       <c r="E76" s="45"/>
       <c r="F76" s="36" t="s">
@@ -8424,10 +8425,10 @@
       <c r="A77" s="35">
         <v>0</v>
       </c>
-      <c r="B77" s="94" t="s">
+      <c r="B77" s="78" t="s">
         <v>138</v>
       </c>
-      <c r="C77" s="94"/>
+      <c r="C77" s="78"/>
       <c r="D77" s="45"/>
       <c r="E77" s="45"/>
       <c r="F77" s="36" t="s">
@@ -8507,10 +8508,10 @@
       <c r="A78" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="B78" s="94" t="s">
+      <c r="B78" s="78" t="s">
         <v>140</v>
       </c>
-      <c r="C78" s="94"/>
+      <c r="C78" s="78"/>
       <c r="D78" s="45"/>
       <c r="E78" s="45"/>
       <c r="F78" s="36" t="s">
@@ -8591,10 +8592,10 @@
       <c r="A79" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="B79" s="94" t="s">
+      <c r="B79" s="78" t="s">
         <v>142</v>
       </c>
-      <c r="C79" s="94"/>
+      <c r="C79" s="78"/>
       <c r="D79" s="45"/>
       <c r="E79" s="45"/>
       <c r="F79" s="36" t="s">
@@ -8675,10 +8676,10 @@
       <c r="A80" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="B80" s="94" t="s">
-        <v>253</v>
-      </c>
-      <c r="C80" s="94"/>
+      <c r="B80" s="78" t="s">
+        <v>252</v>
+      </c>
+      <c r="C80" s="78"/>
       <c r="D80" s="45"/>
       <c r="E80" s="45"/>
       <c r="F80" s="36" t="s">
@@ -8758,10 +8759,10 @@
       <c r="A81" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="B81" s="94" t="s">
+      <c r="B81" s="78" t="s">
         <v>145</v>
       </c>
-      <c r="C81" s="94"/>
+      <c r="C81" s="78"/>
       <c r="D81" s="45"/>
       <c r="E81" s="45"/>
       <c r="F81" s="36" t="s">
@@ -8841,10 +8842,10 @@
       <c r="A82" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="B82" s="94" t="s">
+      <c r="B82" s="78" t="s">
         <v>147</v>
       </c>
-      <c r="C82" s="94"/>
+      <c r="C82" s="78"/>
       <c r="D82" s="45"/>
       <c r="E82" s="45"/>
       <c r="F82" s="36" t="s">
@@ -8925,10 +8926,10 @@
       <c r="A83" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="B83" s="94" t="s">
+      <c r="B83" s="78" t="s">
         <v>149</v>
       </c>
-      <c r="C83" s="94"/>
+      <c r="C83" s="78"/>
       <c r="D83" s="45"/>
       <c r="E83" s="45"/>
       <c r="F83" s="36" t="s">
@@ -9009,10 +9010,10 @@
       <c r="A84" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="B84" s="94" t="s">
+      <c r="B84" s="78" t="s">
         <v>151</v>
       </c>
-      <c r="C84" s="94"/>
+      <c r="C84" s="78"/>
       <c r="D84" s="45"/>
       <c r="E84" s="45"/>
       <c r="F84" s="36" t="s">
@@ -9093,10 +9094,10 @@
       <c r="A85" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="B85" s="94" t="s">
+      <c r="B85" s="78" t="s">
         <v>153</v>
       </c>
-      <c r="C85" s="94"/>
+      <c r="C85" s="78"/>
       <c r="D85" s="45"/>
       <c r="E85" s="45"/>
       <c r="F85" s="36" t="s">
@@ -9177,10 +9178,10 @@
       <c r="A86" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="B86" s="94" t="s">
+      <c r="B86" s="78" t="s">
         <v>155</v>
       </c>
-      <c r="C86" s="94"/>
+      <c r="C86" s="78"/>
       <c r="D86" s="45"/>
       <c r="E86" s="45"/>
       <c r="F86" s="36" t="s">
@@ -9261,10 +9262,10 @@
       <c r="A87" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="B87" s="94" t="s">
+      <c r="B87" s="78" t="s">
         <v>157</v>
       </c>
-      <c r="C87" s="94"/>
+      <c r="C87" s="78"/>
       <c r="D87" s="45"/>
       <c r="E87" s="45"/>
       <c r="F87" s="36" t="s">
@@ -9345,10 +9346,10 @@
       <c r="A88" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="B88" s="94" t="s">
+      <c r="B88" s="78" t="s">
         <v>159</v>
       </c>
-      <c r="C88" s="94"/>
+      <c r="C88" s="78"/>
       <c r="D88" s="45"/>
       <c r="E88" s="45"/>
       <c r="F88" s="36" t="s">
@@ -9428,10 +9429,10 @@
       <c r="A89" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="B89" s="94" t="s">
+      <c r="B89" s="78" t="s">
         <v>161</v>
       </c>
-      <c r="C89" s="94"/>
+      <c r="C89" s="78"/>
       <c r="D89" s="45"/>
       <c r="E89" s="45"/>
       <c r="F89" s="36" t="s">
@@ -9511,10 +9512,10 @@
       <c r="A90" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="B90" s="94" t="s">
-        <v>254</v>
-      </c>
-      <c r="C90" s="94"/>
+      <c r="B90" s="78" t="s">
+        <v>253</v>
+      </c>
+      <c r="C90" s="78"/>
       <c r="D90" s="45"/>
       <c r="E90" s="45"/>
       <c r="F90" s="36" t="s">
@@ -9594,10 +9595,10 @@
       <c r="A91" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="B91" s="94" t="s">
+      <c r="B91" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="94"/>
+      <c r="C91" s="78"/>
       <c r="D91" s="45"/>
       <c r="E91" s="45"/>
       <c r="F91" s="36" t="s">
@@ -9677,10 +9678,10 @@
       <c r="A92" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="B92" s="94" t="s">
+      <c r="B92" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C92" s="94"/>
+      <c r="C92" s="78"/>
       <c r="D92" s="45"/>
       <c r="E92" s="45"/>
       <c r="F92" s="36" t="s">
@@ -9760,10 +9761,10 @@
       <c r="A93" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="B93" s="94" t="s">
+      <c r="B93" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C93" s="94"/>
+      <c r="C93" s="78"/>
       <c r="D93" s="45"/>
       <c r="E93" s="45"/>
       <c r="F93" s="36" t="s">
@@ -9843,10 +9844,10 @@
       <c r="A94" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="B94" s="94" t="s">
+      <c r="B94" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C94" s="94"/>
+      <c r="C94" s="78"/>
       <c r="D94" s="45"/>
       <c r="E94" s="45"/>
       <c r="F94" s="36" t="s">
@@ -9926,10 +9927,10 @@
       <c r="A95" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="B95" s="94" t="s">
+      <c r="B95" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C95" s="94"/>
+      <c r="C95" s="78"/>
       <c r="D95" s="45"/>
       <c r="E95" s="45"/>
       <c r="F95" s="36" t="s">
@@ -10009,10 +10010,10 @@
       <c r="A96" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="B96" s="94" t="s">
+      <c r="B96" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C96" s="94"/>
+      <c r="C96" s="78"/>
       <c r="D96" s="45"/>
       <c r="E96" s="45"/>
       <c r="F96" s="36" t="s">
@@ -10092,10 +10093,10 @@
       <c r="A97" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="B97" s="94" t="s">
+      <c r="B97" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C97" s="94"/>
+      <c r="C97" s="78"/>
       <c r="D97" s="45"/>
       <c r="E97" s="45"/>
       <c r="F97" s="36" t="s">
@@ -10175,10 +10176,10 @@
       <c r="A98" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="B98" s="94" t="s">
+      <c r="B98" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="C98" s="94"/>
+      <c r="C98" s="78"/>
       <c r="D98" s="45"/>
       <c r="E98" s="45"/>
       <c r="F98" s="36" t="s">
@@ -10258,10 +10259,10 @@
       <c r="A99" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="B99" s="94" t="s">
+      <c r="B99" s="78" t="s">
         <v>172</v>
       </c>
-      <c r="C99" s="94"/>
+      <c r="C99" s="78"/>
       <c r="D99" s="45"/>
       <c r="E99" s="45"/>
       <c r="F99" s="36" t="s">
@@ -10341,10 +10342,10 @@
       <c r="A100" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="B100" s="94" t="s">
+      <c r="B100" s="78" t="s">
         <v>174</v>
       </c>
-      <c r="C100" s="94"/>
+      <c r="C100" s="78"/>
       <c r="D100" s="45"/>
       <c r="E100" s="45"/>
       <c r="F100" s="36" t="s">
@@ -10424,10 +10425,10 @@
       <c r="A101" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="B101" s="99" t="s">
+      <c r="B101" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="C101" s="99"/>
+      <c r="C101" s="79"/>
       <c r="D101" s="45"/>
       <c r="E101" s="45"/>
       <c r="F101" s="36" t="s">
@@ -10507,10 +10508,10 @@
       <c r="A102" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="B102" s="94" t="s">
+      <c r="B102" s="78" t="s">
         <v>178</v>
       </c>
-      <c r="C102" s="94"/>
+      <c r="C102" s="78"/>
       <c r="D102" s="45"/>
       <c r="E102" s="45"/>
       <c r="F102" s="36" t="s">
@@ -10590,10 +10591,10 @@
       <c r="A103" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="B103" s="94" t="s">
+      <c r="B103" s="78" t="s">
         <v>180</v>
       </c>
-      <c r="C103" s="94"/>
+      <c r="C103" s="78"/>
       <c r="D103" s="45"/>
       <c r="E103" s="45"/>
       <c r="F103" s="36" t="s">
@@ -10673,10 +10674,10 @@
       <c r="A104" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="B104" s="94" t="s">
+      <c r="B104" s="78" t="s">
         <v>182</v>
       </c>
-      <c r="C104" s="94"/>
+      <c r="C104" s="78"/>
       <c r="D104" s="45"/>
       <c r="E104" s="45"/>
       <c r="F104" s="36" t="s">
@@ -10756,10 +10757,10 @@
       <c r="A105" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="B105" s="94" t="s">
+      <c r="B105" s="78" t="s">
         <v>184</v>
       </c>
-      <c r="C105" s="94"/>
+      <c r="C105" s="78"/>
       <c r="D105" s="45"/>
       <c r="E105" s="45"/>
       <c r="F105" s="36" t="s">
@@ -10839,10 +10840,10 @@
       <c r="A106" s="35" t="s">
         <v>185</v>
       </c>
-      <c r="B106" s="94" t="s">
+      <c r="B106" s="78" t="s">
         <v>186</v>
       </c>
-      <c r="C106" s="94"/>
+      <c r="C106" s="78"/>
       <c r="D106" s="45"/>
       <c r="E106" s="45"/>
       <c r="F106" s="36" t="s">
@@ -10922,10 +10923,10 @@
       <c r="A107" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="B107" s="94" t="s">
+      <c r="B107" s="78" t="s">
         <v>188</v>
       </c>
-      <c r="C107" s="94"/>
+      <c r="C107" s="78"/>
       <c r="D107" s="45"/>
       <c r="E107" s="45"/>
       <c r="F107" s="36" t="s">
@@ -11005,10 +11006,10 @@
       <c r="A108" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="B108" s="99" t="s">
+      <c r="B108" s="79" t="s">
         <v>190</v>
       </c>
-      <c r="C108" s="99"/>
+      <c r="C108" s="79"/>
       <c r="D108" s="45"/>
       <c r="E108" s="45"/>
       <c r="F108" s="36" t="s">
@@ -11088,10 +11089,10 @@
       <c r="A109" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="B109" s="99" t="s">
+      <c r="B109" s="79" t="s">
         <v>190</v>
       </c>
-      <c r="C109" s="99"/>
+      <c r="C109" s="79"/>
       <c r="D109" s="45"/>
       <c r="E109" s="45"/>
       <c r="F109" s="36" t="s">
@@ -11171,10 +11172,10 @@
       <c r="A110" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="B110" s="99" t="s">
+      <c r="B110" s="79" t="s">
         <v>190</v>
       </c>
-      <c r="C110" s="99"/>
+      <c r="C110" s="79"/>
       <c r="D110" s="45"/>
       <c r="E110" s="45"/>
       <c r="F110" s="36" t="s">
@@ -11254,10 +11255,10 @@
       <c r="A111" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="B111" s="99" t="s">
+      <c r="B111" s="79" t="s">
         <v>190</v>
       </c>
-      <c r="C111" s="99"/>
+      <c r="C111" s="79"/>
       <c r="D111" s="45"/>
       <c r="E111" s="45"/>
       <c r="F111" s="36" t="s">
@@ -11337,10 +11338,10 @@
       <c r="A112" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="B112" s="99" t="s">
+      <c r="B112" s="79" t="s">
         <v>190</v>
       </c>
-      <c r="C112" s="99"/>
+      <c r="C112" s="79"/>
       <c r="D112" s="45"/>
       <c r="E112" s="45"/>
       <c r="F112" s="36" t="s">
@@ -11420,10 +11421,10 @@
       <c r="A113" s="35" t="s">
         <v>195</v>
       </c>
-      <c r="B113" s="99" t="s">
+      <c r="B113" s="79" t="s">
         <v>190</v>
       </c>
-      <c r="C113" s="99"/>
+      <c r="C113" s="79"/>
       <c r="D113" s="45"/>
       <c r="E113" s="45"/>
       <c r="F113" s="36" t="s">
@@ -11503,10 +11504,10 @@
       <c r="A114" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="B114" s="99" t="s">
+      <c r="B114" s="79" t="s">
         <v>190</v>
       </c>
-      <c r="C114" s="99"/>
+      <c r="C114" s="79"/>
       <c r="D114" s="45"/>
       <c r="E114" s="45"/>
       <c r="F114" s="36" t="s">
@@ -11586,10 +11587,10 @@
       <c r="A115" s="35" t="s">
         <v>197</v>
       </c>
-      <c r="B115" s="94" t="s">
+      <c r="B115" s="78" t="s">
         <v>198</v>
       </c>
-      <c r="C115" s="94"/>
+      <c r="C115" s="78"/>
       <c r="D115" s="45"/>
       <c r="E115" s="45"/>
       <c r="F115" s="36" t="s">
@@ -11669,10 +11670,10 @@
       <c r="A116" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="B116" s="94" t="s">
+      <c r="B116" s="78" t="s">
         <v>200</v>
       </c>
-      <c r="C116" s="94"/>
+      <c r="C116" s="78"/>
       <c r="D116" s="45"/>
       <c r="E116" s="45"/>
       <c r="F116" s="36" t="s">
@@ -11752,10 +11753,10 @@
       <c r="A117" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="B117" s="94" t="s">
+      <c r="B117" s="78" t="s">
         <v>202</v>
       </c>
-      <c r="C117" s="94"/>
+      <c r="C117" s="78"/>
       <c r="D117" s="45"/>
       <c r="E117" s="45"/>
       <c r="F117" s="36" t="s">
@@ -11835,10 +11836,10 @@
       <c r="A118" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="B118" s="94" t="s">
+      <c r="B118" s="78" t="s">
         <v>204</v>
       </c>
-      <c r="C118" s="94"/>
+      <c r="C118" s="78"/>
       <c r="D118" s="45"/>
       <c r="E118" s="45"/>
       <c r="F118" s="36" t="s">
@@ -11918,10 +11919,10 @@
       <c r="A119" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="B119" s="94" t="s">
+      <c r="B119" s="78" t="s">
         <v>206</v>
       </c>
-      <c r="C119" s="94"/>
+      <c r="C119" s="78"/>
       <c r="D119" s="45"/>
       <c r="E119" s="45"/>
       <c r="F119" s="36" t="s">
@@ -12002,10 +12003,10 @@
       <c r="A120" s="35" t="s">
         <v>207</v>
       </c>
-      <c r="B120" s="94" t="s">
+      <c r="B120" s="78" t="s">
         <v>208</v>
       </c>
-      <c r="C120" s="94"/>
+      <c r="C120" s="78"/>
       <c r="D120" s="45"/>
       <c r="E120" s="45"/>
       <c r="F120" s="36" t="s">
@@ -12086,10 +12087,10 @@
       <c r="A121" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="B121" s="94" t="s">
+      <c r="B121" s="78" t="s">
         <v>210</v>
       </c>
-      <c r="C121" s="94"/>
+      <c r="C121" s="78"/>
       <c r="D121" s="45"/>
       <c r="E121" s="45"/>
       <c r="F121" s="36" t="s">
@@ -12169,10 +12170,10 @@
       <c r="A122" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="B122" s="94" t="s">
+      <c r="B122" s="78" t="s">
         <v>212</v>
       </c>
-      <c r="C122" s="94"/>
+      <c r="C122" s="78"/>
       <c r="D122" s="45"/>
       <c r="E122" s="45"/>
       <c r="F122" s="36" t="s">
@@ -12252,10 +12253,10 @@
       <c r="A123" s="35" t="s">
         <v>213</v>
       </c>
-      <c r="B123" s="94" t="s">
+      <c r="B123" s="78" t="s">
         <v>214</v>
       </c>
-      <c r="C123" s="94"/>
+      <c r="C123" s="78"/>
       <c r="D123" s="45"/>
       <c r="E123" s="45"/>
       <c r="F123" s="36" t="s">
@@ -12335,10 +12336,10 @@
       <c r="A124" s="35" t="s">
         <v>215</v>
       </c>
-      <c r="B124" s="94" t="s">
+      <c r="B124" s="78" t="s">
         <v>216</v>
       </c>
-      <c r="C124" s="94"/>
+      <c r="C124" s="78"/>
       <c r="D124" s="45"/>
       <c r="E124" s="45"/>
       <c r="F124" s="36" t="s">
@@ -12418,10 +12419,10 @@
       <c r="A125" s="35" t="s">
         <v>217</v>
       </c>
-      <c r="B125" s="94" t="s">
+      <c r="B125" s="78" t="s">
         <v>218</v>
       </c>
-      <c r="C125" s="94"/>
+      <c r="C125" s="78"/>
       <c r="D125" s="45"/>
       <c r="E125" s="45"/>
       <c r="F125" s="36" t="s">
@@ -12501,10 +12502,10 @@
       <c r="A126" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="B126" s="94" t="s">
+      <c r="B126" s="78" t="s">
         <v>220</v>
       </c>
-      <c r="C126" s="94"/>
+      <c r="C126" s="78"/>
       <c r="D126" s="45"/>
       <c r="E126" s="45"/>
       <c r="F126" s="36" t="s">
@@ -12584,10 +12585,10 @@
       <c r="A127" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="B127" s="94" t="s">
+      <c r="B127" s="78" t="s">
         <v>222</v>
       </c>
-      <c r="C127" s="94"/>
+      <c r="C127" s="78"/>
       <c r="D127" s="45"/>
       <c r="E127" s="45"/>
       <c r="F127" s="36" t="s">
@@ -12667,10 +12668,10 @@
       <c r="A128" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="B128" s="94" t="s">
+      <c r="B128" s="78" t="s">
         <v>224</v>
       </c>
-      <c r="C128" s="94"/>
+      <c r="C128" s="78"/>
       <c r="D128" s="45"/>
       <c r="E128" s="45"/>
       <c r="F128" s="36" t="s">
@@ -12750,10 +12751,10 @@
       <c r="A129" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="B129" s="94" t="s">
+      <c r="B129" s="78" t="s">
         <v>226</v>
       </c>
-      <c r="C129" s="94"/>
+      <c r="C129" s="78"/>
       <c r="D129" s="45"/>
       <c r="E129" s="45"/>
       <c r="F129" s="36" t="s">
@@ -12833,10 +12834,10 @@
       <c r="A130" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="B130" s="94" t="s">
+      <c r="B130" s="78" t="s">
         <v>228</v>
       </c>
-      <c r="C130" s="94"/>
+      <c r="C130" s="78"/>
       <c r="D130" s="45"/>
       <c r="E130" s="45"/>
       <c r="F130" s="36" t="s">
@@ -12916,10 +12917,10 @@
       <c r="A131" s="35" t="s">
         <v>229</v>
       </c>
-      <c r="B131" s="91" t="s">
+      <c r="B131" s="77" t="s">
         <v>230</v>
       </c>
-      <c r="C131" s="91"/>
+      <c r="C131" s="77"/>
       <c r="D131" s="36"/>
       <c r="E131" s="36"/>
       <c r="F131" s="36" t="s">
@@ -13230,7 +13231,7 @@
       <c r="D132" s="55"/>
       <c r="E132" s="49"/>
       <c r="F132" s="56" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="G132" s="49"/>
       <c r="H132" s="57"/>
@@ -13256,7 +13257,7 @@
     </row>
     <row r="133" spans="1:255" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A133" s="63" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B133" s="64"/>
       <c r="C133" s="65"/>
@@ -13283,7 +13284,7 @@
     </row>
     <row r="134" spans="1:255" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134" s="76" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B134" s="67"/>
       <c r="C134" s="2"/>
@@ -13310,7 +13311,7 @@
     </row>
     <row r="135" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="76" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B135" s="67"/>
       <c r="C135" s="2"/>
@@ -13337,7 +13338,7 @@
     </row>
     <row r="136" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="63" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B136" s="67"/>
       <c r="C136" s="2"/>
@@ -13364,7 +13365,7 @@
     </row>
     <row r="137" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="63" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B137" s="67"/>
       <c r="C137" s="2"/>
@@ -13391,7 +13392,7 @@
     </row>
     <row r="138" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="63" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B138" s="67"/>
       <c r="C138" s="2"/>
@@ -13418,7 +13419,7 @@
     </row>
     <row r="139" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="63" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B139" s="67"/>
       <c r="C139" s="2"/>
@@ -13445,7 +13446,7 @@
     </row>
     <row r="140" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="63" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B140" s="67"/>
       <c r="C140" s="2"/>
@@ -13472,7 +13473,7 @@
     </row>
     <row r="141" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="63" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B141" s="67"/>
       <c r="C141" s="2"/>
@@ -13499,7 +13500,7 @@
     </row>
     <row r="142" spans="1:255" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="63" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B142" s="67"/>
       <c r="C142" s="2"/>
@@ -13526,7 +13527,7 @@
     </row>
     <row r="143" spans="1:255" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143" s="76" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B143" s="64"/>
       <c r="C143" s="65"/>
@@ -13548,7 +13549,7 @@
     </row>
     <row r="144" spans="1:255" s="61" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="76" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B144" s="64"/>
       <c r="C144" s="65"/>
@@ -13575,7 +13576,7 @@
     </row>
     <row r="145" spans="1:46" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="76" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B145" s="71"/>
       <c r="C145" s="72"/>
@@ -13602,7 +13603,7 @@
     </row>
     <row r="146" spans="1:46" s="61" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="76" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B146" s="64"/>
       <c r="C146" s="65"/>
@@ -13629,7 +13630,7 @@
     </row>
     <row r="147" spans="1:46" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="76" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B147" s="64"/>
       <c r="C147" s="65"/>
@@ -13656,7 +13657,7 @@
     </row>
     <row r="148" spans="1:46" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="76" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B148" s="64"/>
       <c r="C148" s="65"/>
@@ -14185,133 +14186,6 @@
     </row>
   </sheetData>
   <mergeCells count="141">
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A2:U2"/>
     <mergeCell ref="J5:K5"/>
@@ -14326,6 +14200,133 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:S7"/>
     <mergeCell ref="T7:U7"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="B130:C130"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Update dailyreport template itemname
之前曾經將珍珠拔修改為珍珠芭,
後因網路查詢為珍珠拔,又將名稱改回珍珠拔,
本次依昭蓉轉達徐主任意思,將珍珠拔的名稱修改為珍珠芭
</commit_message>
<xml_diff>
--- a/src/apps/dailytrans/reports/template.xlsx
+++ b/src/apps/dailytrans/reports/template.xlsx
@@ -1450,16 +1450,16 @@
     <phoneticPr fontId="26" type="noConversion"/>
   </si>
   <si>
-    <t>珍珠拔</t>
-    <phoneticPr fontId="26" type="noConversion"/>
-  </si>
-  <si>
     <t>鳳梨釋迦
 (產地)</t>
     <phoneticPr fontId="26" type="noConversion"/>
   </si>
   <si>
     <t>表該產品最近連續一週價格低或高於監控價格；</t>
+    <phoneticPr fontId="26" type="noConversion"/>
+  </si>
+  <si>
+    <t>珍珠芭</t>
     <phoneticPr fontId="26" type="noConversion"/>
   </si>
 </sst>
@@ -2030,36 +2030,6 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="21" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2098,6 +2068,36 @@
     </xf>
     <xf numFmtId="179" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="21" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2475,8 +2475,8 @@
   <dimension ref="A1:AMJ256"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M132" sqref="M132"/>
+      <pane ySplit="8" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B80" sqref="B80:C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
@@ -2510,35 +2510,35 @@
       <c r="F1" s="8"/>
       <c r="G1" s="9"/>
       <c r="H1" s="10"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
       <c r="M1" s="11"/>
       <c r="N1" s="11"/>
     </row>
     <row r="2" spans="1:30" s="12" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="88"/>
-      <c r="H2" s="88"/>
-      <c r="I2" s="88"/>
-      <c r="J2" s="88"/>
-      <c r="K2" s="88"/>
-      <c r="L2" s="88"/>
-      <c r="M2" s="88"/>
-      <c r="N2" s="88"/>
-      <c r="O2" s="88"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="88"/>
-      <c r="S2" s="88"/>
-      <c r="T2" s="88"/>
-      <c r="U2" s="88"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="78"/>
+      <c r="N2" s="78"/>
+      <c r="O2" s="78"/>
+      <c r="P2" s="78"/>
+      <c r="Q2" s="78"/>
+      <c r="R2" s="78"/>
+      <c r="S2" s="78"/>
+      <c r="T2" s="78"/>
+      <c r="U2" s="78"/>
     </row>
     <row r="3" spans="1:30" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="13"/>
@@ -2587,8 +2587,8 @@
       <c r="G5" s="20"/>
       <c r="H5" s="21"/>
       <c r="I5" s="22"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
       <c r="L5" s="21"/>
       <c r="M5" s="23"/>
       <c r="N5" s="23"/>
@@ -2597,41 +2597,41 @@
       <c r="S5" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="T5" s="90" t="s">
+      <c r="T5" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="U5" s="90"/>
+      <c r="U5" s="80"/>
     </row>
     <row r="6" spans="1:30" s="12" customFormat="1" ht="31.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="91" t="s">
+      <c r="A6" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="94" t="s">
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="95" t="s">
+      <c r="G6" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="91" t="s">
+      <c r="H6" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="91"/>
-      <c r="J6" s="91"/>
-      <c r="K6" s="91"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="91"/>
-      <c r="N6" s="91"/>
-      <c r="O6" s="91"/>
-      <c r="P6" s="91"/>
-      <c r="Q6" s="91"/>
-      <c r="R6" s="91"/>
-      <c r="S6" s="91"/>
-      <c r="T6" s="91"/>
-      <c r="U6" s="91"/>
+      <c r="I6" s="81"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
+      <c r="N6" s="81"/>
+      <c r="O6" s="81"/>
+      <c r="P6" s="81"/>
+      <c r="Q6" s="81"/>
+      <c r="R6" s="81"/>
+      <c r="S6" s="81"/>
+      <c r="T6" s="81"/>
+      <c r="U6" s="81"/>
       <c r="V6" s="1"/>
       <c r="W6" s="28"/>
       <c r="X6" s="28"/>
@@ -2643,36 +2643,36 @@
       <c r="AD6" s="28"/>
     </row>
     <row r="7" spans="1:30" s="12" customFormat="1" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="91"/>
-      <c r="B7" s="91"/>
-      <c r="C7" s="91"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="96" t="s">
+      <c r="A7" s="81"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="81"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="86" t="s">
         <v>7</v>
       </c>
       <c r="I7" s="29"/>
       <c r="J7" s="29"/>
       <c r="K7" s="29"/>
-      <c r="L7" s="97" t="s">
+      <c r="L7" s="87" t="s">
         <v>245</v>
       </c>
-      <c r="M7" s="98" t="s">
+      <c r="M7" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="98"/>
-      <c r="O7" s="98"/>
-      <c r="P7" s="98"/>
-      <c r="Q7" s="98"/>
-      <c r="R7" s="98"/>
-      <c r="S7" s="98"/>
-      <c r="T7" s="99" t="s">
+      <c r="N7" s="88"/>
+      <c r="O7" s="88"/>
+      <c r="P7" s="88"/>
+      <c r="Q7" s="88"/>
+      <c r="R7" s="88"/>
+      <c r="S7" s="88"/>
+      <c r="T7" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="U7" s="99"/>
-      <c r="V7" s="84"/>
+      <c r="U7" s="89"/>
+      <c r="V7" s="90"/>
       <c r="W7" s="30"/>
       <c r="X7" s="30"/>
       <c r="Y7" s="30"/>
@@ -2683,14 +2683,14 @@
       <c r="AD7" s="30"/>
     </row>
     <row r="8" spans="1:30" s="12" customFormat="1" ht="49.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="91"/>
-      <c r="B8" s="91"/>
-      <c r="C8" s="91"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="95"/>
-      <c r="H8" s="96"/>
+      <c r="A8" s="81"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="83"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="86"/>
       <c r="I8" s="31" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -2703,7 +2703,7 @@
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="L8" s="97"/>
+      <c r="L8" s="87"/>
       <c r="M8" s="32" t="s">
         <v>246</v>
       </c>
@@ -2731,7 +2731,7 @@
       <c r="U8" s="33" t="s">
         <v>247</v>
       </c>
-      <c r="V8" s="84"/>
+      <c r="V8" s="90"/>
       <c r="W8" s="34" t="s">
         <v>12</v>
       </c>
@@ -2761,13 +2761,13 @@
       <c r="A9" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="91" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="77"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="86" t="s">
+      <c r="C9" s="91"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="93" t="s">
         <v>15</v>
       </c>
       <c r="G9" s="37" t="s">
@@ -2844,13 +2844,13 @@
       <c r="A10" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="77"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="85"/>
-      <c r="F10" s="85"/>
+      <c r="C10" s="91"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="92"/>
       <c r="G10" s="37" t="s">
         <v>15</v>
       </c>
@@ -2925,10 +2925,10 @@
       <c r="A11" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="77"/>
+      <c r="C11" s="91"/>
       <c r="D11" s="36" t="s">
         <v>15</v>
       </c>
@@ -3012,10 +3012,10 @@
       <c r="A12" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="77" t="s">
+      <c r="B12" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="77"/>
+      <c r="C12" s="91"/>
       <c r="D12" s="36" t="s">
         <v>15</v>
       </c>
@@ -3099,10 +3099,10 @@
       <c r="A13" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="91" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="77"/>
+      <c r="C13" s="91"/>
       <c r="D13" s="36" t="s">
         <v>15</v>
       </c>
@@ -3186,10 +3186,10 @@
       <c r="A14" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="78" t="s">
+      <c r="B14" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="78"/>
+      <c r="C14" s="94"/>
       <c r="D14" s="43"/>
       <c r="E14" s="43"/>
       <c r="F14" s="36" t="s">
@@ -3270,10 +3270,10 @@
       <c r="A15" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="78" t="s">
+      <c r="B15" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="78"/>
+      <c r="C15" s="94"/>
       <c r="D15" s="43"/>
       <c r="E15" s="43"/>
       <c r="F15" s="36" t="s">
@@ -3353,10 +3353,10 @@
       <c r="A16" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="78" t="s">
+      <c r="B16" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="78"/>
+      <c r="C16" s="94"/>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
       <c r="F16" s="36" t="s">
@@ -3436,10 +3436,10 @@
       <c r="A17" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="78" t="s">
+      <c r="B17" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="78"/>
+      <c r="C17" s="94"/>
       <c r="D17" s="43"/>
       <c r="E17" s="43"/>
       <c r="F17" s="36" t="s">
@@ -3519,10 +3519,10 @@
       <c r="A18" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="83" t="s">
+      <c r="B18" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="83"/>
+      <c r="C18" s="95"/>
       <c r="D18" s="43"/>
       <c r="E18" s="43"/>
       <c r="F18" s="36" t="s">
@@ -3602,10 +3602,10 @@
       <c r="A19" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="78" t="s">
+      <c r="B19" s="94" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="78"/>
+      <c r="C19" s="94"/>
       <c r="D19" s="43"/>
       <c r="E19" s="43"/>
       <c r="F19" s="36" t="s">
@@ -3685,10 +3685,10 @@
       <c r="A20" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="78" t="s">
+      <c r="B20" s="94" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="78"/>
+      <c r="C20" s="94"/>
       <c r="D20" s="43"/>
       <c r="E20" s="43"/>
       <c r="F20" s="36" t="s">
@@ -3768,10 +3768,10 @@
       <c r="A21" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="78" t="s">
+      <c r="B21" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="78"/>
+      <c r="C21" s="94"/>
       <c r="D21" s="43"/>
       <c r="E21" s="43"/>
       <c r="F21" s="36" t="s">
@@ -3851,10 +3851,10 @@
       <c r="A22" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="78" t="s">
+      <c r="B22" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="78"/>
+      <c r="C22" s="94"/>
       <c r="D22" s="43"/>
       <c r="E22" s="43"/>
       <c r="F22" s="36" t="s">
@@ -3934,10 +3934,10 @@
       <c r="A23" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="78" t="s">
+      <c r="B23" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="78"/>
+      <c r="C23" s="94"/>
       <c r="D23" s="43"/>
       <c r="E23" s="43"/>
       <c r="F23" s="36" t="s">
@@ -4017,10 +4017,10 @@
       <c r="A24" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="78" t="s">
+      <c r="B24" s="94" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="78"/>
+      <c r="C24" s="94"/>
       <c r="D24" s="43"/>
       <c r="E24" s="43"/>
       <c r="F24" s="36" t="s">
@@ -4100,10 +4100,10 @@
       <c r="A25" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="83" t="s">
+      <c r="B25" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="83"/>
+      <c r="C25" s="95"/>
       <c r="D25" s="43"/>
       <c r="E25" s="43"/>
       <c r="F25" s="36" t="s">
@@ -4183,10 +4183,10 @@
       <c r="A26" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="78" t="s">
+      <c r="B26" s="94" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="78"/>
+      <c r="C26" s="94"/>
       <c r="D26" s="43"/>
       <c r="E26" s="43"/>
       <c r="F26" s="36" t="s">
@@ -4266,10 +4266,10 @@
       <c r="A27" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="78" t="s">
+      <c r="B27" s="94" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="78"/>
+      <c r="C27" s="94"/>
       <c r="D27" s="43"/>
       <c r="E27" s="43"/>
       <c r="F27" s="36" t="s">
@@ -4349,10 +4349,10 @@
       <c r="A28" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="78" t="s">
+      <c r="B28" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="78"/>
+      <c r="C28" s="94"/>
       <c r="D28" s="43"/>
       <c r="E28" s="43"/>
       <c r="F28" s="36" t="s">
@@ -4432,10 +4432,10 @@
       <c r="A29" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="83" t="s">
+      <c r="B29" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="83"/>
+      <c r="C29" s="95"/>
       <c r="D29" s="43"/>
       <c r="E29" s="43"/>
       <c r="F29" s="36" t="s">
@@ -4516,10 +4516,10 @@
       <c r="A30" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="83" t="s">
+      <c r="B30" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="83"/>
+      <c r="C30" s="95"/>
       <c r="D30" s="43"/>
       <c r="E30" s="43"/>
       <c r="F30" s="36" t="s">
@@ -4600,10 +4600,10 @@
       <c r="A31" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="78" t="s">
+      <c r="B31" s="94" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="78"/>
+      <c r="C31" s="94"/>
       <c r="D31" s="43"/>
       <c r="E31" s="43"/>
       <c r="F31" s="36" t="s">
@@ -4683,10 +4683,10 @@
       <c r="A32" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="78" t="s">
+      <c r="B32" s="94" t="s">
         <v>62</v>
       </c>
-      <c r="C32" s="78"/>
+      <c r="C32" s="94"/>
       <c r="D32" s="43"/>
       <c r="E32" s="43"/>
       <c r="F32" s="36" t="s">
@@ -4766,10 +4766,10 @@
       <c r="A33" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="78" t="s">
+      <c r="B33" s="94" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="78"/>
+      <c r="C33" s="94"/>
       <c r="D33" s="45"/>
       <c r="E33" s="45"/>
       <c r="F33" s="36" t="s">
@@ -4850,10 +4850,10 @@
       <c r="A34" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="B34" s="78" t="s">
+      <c r="B34" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="C34" s="78"/>
+      <c r="C34" s="94"/>
       <c r="D34" s="45"/>
       <c r="E34" s="45"/>
       <c r="F34" s="36" t="s">
@@ -4933,10 +4933,10 @@
       <c r="A35" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="78" t="s">
+      <c r="B35" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="78"/>
+      <c r="C35" s="94"/>
       <c r="D35" s="45"/>
       <c r="E35" s="45"/>
       <c r="F35" s="36" t="s">
@@ -5016,10 +5016,10 @@
       <c r="A36" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="B36" s="78" t="s">
+      <c r="B36" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="78"/>
+      <c r="C36" s="94"/>
       <c r="D36" s="45"/>
       <c r="E36" s="45"/>
       <c r="F36" s="36" t="s">
@@ -5099,10 +5099,10 @@
       <c r="A37" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="B37" s="78" t="s">
+      <c r="B37" s="94" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="78"/>
+      <c r="C37" s="94"/>
       <c r="D37" s="45"/>
       <c r="E37" s="45"/>
       <c r="F37" s="36" t="s">
@@ -5182,10 +5182,10 @@
       <c r="A38" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="78" t="s">
+      <c r="B38" s="94" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="78"/>
+      <c r="C38" s="94"/>
       <c r="D38" s="45"/>
       <c r="E38" s="45"/>
       <c r="F38" s="36" t="s">
@@ -5265,10 +5265,10 @@
       <c r="A39" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="78" t="s">
+      <c r="B39" s="94" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="78"/>
+      <c r="C39" s="94"/>
       <c r="D39" s="45"/>
       <c r="E39" s="45"/>
       <c r="F39" s="36" t="s">
@@ -5348,10 +5348,10 @@
       <c r="A40" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="78" t="s">
+      <c r="B40" s="94" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="78"/>
+      <c r="C40" s="94"/>
       <c r="D40" s="45"/>
       <c r="E40" s="45"/>
       <c r="F40" s="36" t="s">
@@ -5431,10 +5431,10 @@
       <c r="A41" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="B41" s="78" t="s">
+      <c r="B41" s="94" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="78"/>
+      <c r="C41" s="94"/>
       <c r="D41" s="45"/>
       <c r="E41" s="45"/>
       <c r="F41" s="36" t="s">
@@ -5514,10 +5514,10 @@
       <c r="A42" s="35" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="78" t="s">
+      <c r="B42" s="94" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="78"/>
+      <c r="C42" s="94"/>
       <c r="D42" s="45"/>
       <c r="E42" s="45"/>
       <c r="F42" s="36" t="s">
@@ -5598,10 +5598,10 @@
       <c r="A43" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="B43" s="82" t="s">
+      <c r="B43" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="C43" s="82"/>
+      <c r="C43" s="96"/>
       <c r="D43" s="45"/>
       <c r="E43" s="45"/>
       <c r="F43" s="36" t="s">
@@ -5681,10 +5681,10 @@
       <c r="A44" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="82" t="s">
+      <c r="B44" s="96" t="s">
         <v>86</v>
       </c>
-      <c r="C44" s="82"/>
+      <c r="C44" s="96"/>
       <c r="D44" s="45"/>
       <c r="E44" s="45"/>
       <c r="F44" s="36" t="s">
@@ -5764,10 +5764,10 @@
       <c r="A45" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="B45" s="78" t="s">
+      <c r="B45" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C45" s="78"/>
+      <c r="C45" s="94"/>
       <c r="D45" s="45"/>
       <c r="E45" s="45"/>
       <c r="F45" s="36" t="s">
@@ -5847,10 +5847,10 @@
       <c r="A46" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="B46" s="78" t="s">
+      <c r="B46" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="78"/>
+      <c r="C46" s="94"/>
       <c r="D46" s="45"/>
       <c r="E46" s="45"/>
       <c r="F46" s="36" t="s">
@@ -5930,10 +5930,10 @@
       <c r="A47" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="B47" s="78" t="s">
+      <c r="B47" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C47" s="78"/>
+      <c r="C47" s="94"/>
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
       <c r="F47" s="36" t="s">
@@ -6013,10 +6013,10 @@
       <c r="A48" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="78" t="s">
+      <c r="B48" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C48" s="78"/>
+      <c r="C48" s="94"/>
       <c r="D48" s="45"/>
       <c r="E48" s="45"/>
       <c r="F48" s="36" t="s">
@@ -6096,10 +6096,10 @@
       <c r="A49" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="B49" s="78" t="s">
+      <c r="B49" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C49" s="78"/>
+      <c r="C49" s="94"/>
       <c r="D49" s="45"/>
       <c r="E49" s="45"/>
       <c r="F49" s="36" t="s">
@@ -6179,10 +6179,10 @@
       <c r="A50" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="B50" s="78" t="s">
+      <c r="B50" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C50" s="78"/>
+      <c r="C50" s="94"/>
       <c r="D50" s="45"/>
       <c r="E50" s="45"/>
       <c r="F50" s="36" t="s">
@@ -6262,10 +6262,10 @@
       <c r="A51" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="78" t="s">
+      <c r="B51" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C51" s="78"/>
+      <c r="C51" s="94"/>
       <c r="D51" s="45"/>
       <c r="E51" s="45"/>
       <c r="F51" s="36" t="s">
@@ -6345,10 +6345,10 @@
       <c r="A52" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="78" t="s">
+      <c r="B52" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C52" s="78"/>
+      <c r="C52" s="94"/>
       <c r="D52" s="45"/>
       <c r="E52" s="45"/>
       <c r="F52" s="36" t="s">
@@ -6428,10 +6428,10 @@
       <c r="A53" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="B53" s="78" t="s">
+      <c r="B53" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C53" s="78"/>
+      <c r="C53" s="94"/>
       <c r="D53" s="45"/>
       <c r="E53" s="45"/>
       <c r="F53" s="36" t="s">
@@ -6511,10 +6511,10 @@
       <c r="A54" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="B54" s="78" t="s">
+      <c r="B54" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C54" s="78"/>
+      <c r="C54" s="94"/>
       <c r="D54" s="45"/>
       <c r="E54" s="45"/>
       <c r="F54" s="36" t="s">
@@ -6594,10 +6594,10 @@
       <c r="A55" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="B55" s="78" t="s">
+      <c r="B55" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C55" s="78"/>
+      <c r="C55" s="94"/>
       <c r="D55" s="45"/>
       <c r="E55" s="45"/>
       <c r="F55" s="36" t="s">
@@ -6677,10 +6677,10 @@
       <c r="A56" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="B56" s="78" t="s">
+      <c r="B56" s="94" t="s">
         <v>100</v>
       </c>
-      <c r="C56" s="78"/>
+      <c r="C56" s="94"/>
       <c r="D56" s="45"/>
       <c r="E56" s="45"/>
       <c r="F56" s="36" t="s">
@@ -6760,10 +6760,10 @@
       <c r="A57" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="B57" s="78" t="s">
+      <c r="B57" s="94" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="78"/>
+      <c r="C57" s="94"/>
       <c r="D57" s="45"/>
       <c r="E57" s="45"/>
       <c r="F57" s="36" t="s">
@@ -6843,10 +6843,10 @@
       <c r="A58" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="B58" s="78" t="s">
+      <c r="B58" s="94" t="s">
         <v>104</v>
       </c>
-      <c r="C58" s="78"/>
+      <c r="C58" s="94"/>
       <c r="D58" s="45"/>
       <c r="E58" s="45"/>
       <c r="F58" s="36" t="s">
@@ -6926,10 +6926,10 @@
       <c r="A59" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="B59" s="78" t="s">
+      <c r="B59" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="C59" s="78"/>
+      <c r="C59" s="94"/>
       <c r="D59" s="45"/>
       <c r="E59" s="45"/>
       <c r="F59" s="36" t="s">
@@ -7009,10 +7009,10 @@
       <c r="A60" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="B60" s="78" t="s">
+      <c r="B60" s="94" t="s">
         <v>108</v>
       </c>
-      <c r="C60" s="78"/>
+      <c r="C60" s="94"/>
       <c r="D60" s="45"/>
       <c r="E60" s="45"/>
       <c r="F60" s="36" t="s">
@@ -7092,10 +7092,10 @@
       <c r="A61" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="B61" s="78" t="s">
+      <c r="B61" s="94" t="s">
         <v>110</v>
       </c>
-      <c r="C61" s="78"/>
+      <c r="C61" s="94"/>
       <c r="D61" s="45"/>
       <c r="E61" s="45"/>
       <c r="F61" s="36" t="s">
@@ -7175,10 +7175,10 @@
       <c r="A62" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="B62" s="78" t="s">
+      <c r="B62" s="94" t="s">
         <v>112</v>
       </c>
-      <c r="C62" s="78"/>
+      <c r="C62" s="94"/>
       <c r="D62" s="45"/>
       <c r="E62" s="45"/>
       <c r="F62" s="36" t="s">
@@ -7259,10 +7259,10 @@
       <c r="A63" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="B63" s="78" t="s">
+      <c r="B63" s="94" t="s">
         <v>251</v>
       </c>
-      <c r="C63" s="78"/>
+      <c r="C63" s="94"/>
       <c r="D63" s="45"/>
       <c r="E63" s="45"/>
       <c r="F63" s="36" t="s">
@@ -7342,10 +7342,10 @@
       <c r="A64" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="B64" s="78" t="s">
+      <c r="B64" s="94" t="s">
         <v>115</v>
       </c>
-      <c r="C64" s="78"/>
+      <c r="C64" s="94"/>
       <c r="D64" s="45"/>
       <c r="E64" s="45"/>
       <c r="F64" s="36" t="s">
@@ -7426,10 +7426,10 @@
       <c r="A65" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="B65" s="78" t="s">
+      <c r="B65" s="94" t="s">
         <v>117</v>
       </c>
-      <c r="C65" s="78"/>
+      <c r="C65" s="94"/>
       <c r="D65" s="45"/>
       <c r="E65" s="45"/>
       <c r="F65" s="36" t="s">
@@ -7509,10 +7509,10 @@
       <c r="A66" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="B66" s="78" t="s">
+      <c r="B66" s="94" t="s">
         <v>119</v>
       </c>
-      <c r="C66" s="78"/>
+      <c r="C66" s="94"/>
       <c r="D66" s="45"/>
       <c r="E66" s="45"/>
       <c r="F66" s="36" t="s">
@@ -7593,10 +7593,10 @@
       <c r="A67" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="B67" s="78" t="s">
+      <c r="B67" s="94" t="s">
         <v>121</v>
       </c>
-      <c r="C67" s="78"/>
+      <c r="C67" s="94"/>
       <c r="D67" s="45"/>
       <c r="E67" s="45"/>
       <c r="F67" s="36" t="s">
@@ -7676,10 +7676,10 @@
       <c r="A68" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="B68" s="78" t="s">
+      <c r="B68" s="94" t="s">
         <v>123</v>
       </c>
-      <c r="C68" s="78"/>
+      <c r="C68" s="94"/>
       <c r="D68" s="45"/>
       <c r="E68" s="45"/>
       <c r="F68" s="36" t="s">
@@ -7759,10 +7759,10 @@
       <c r="A69" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="B69" s="78" t="s">
+      <c r="B69" s="94" t="s">
         <v>125</v>
       </c>
-      <c r="C69" s="78"/>
+      <c r="C69" s="94"/>
       <c r="D69" s="45"/>
       <c r="E69" s="45"/>
       <c r="F69" s="36" t="s">
@@ -7843,10 +7843,10 @@
       <c r="A70" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="B70" s="78" t="s">
+      <c r="B70" s="94" t="s">
         <v>127</v>
       </c>
-      <c r="C70" s="78"/>
+      <c r="C70" s="94"/>
       <c r="D70" s="45"/>
       <c r="E70" s="45"/>
       <c r="F70" s="36" t="s">
@@ -7926,10 +7926,10 @@
       <c r="A71" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="B71" s="80" t="s">
+      <c r="B71" s="97" t="s">
         <v>129</v>
       </c>
-      <c r="C71" s="80"/>
+      <c r="C71" s="97"/>
       <c r="D71" s="47"/>
       <c r="E71" s="47"/>
       <c r="F71" s="36" t="s">
@@ -8008,10 +8008,10 @@
     </row>
     <row r="72" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="48"/>
-      <c r="B72" s="78" t="s">
+      <c r="B72" s="94" t="s">
         <v>130</v>
       </c>
-      <c r="C72" s="78"/>
+      <c r="C72" s="94"/>
       <c r="D72" s="45"/>
       <c r="E72" s="45"/>
       <c r="F72" s="36" t="s">
@@ -8090,14 +8090,14 @@
     </row>
     <row r="73" spans="1:30" s="12" customFormat="1" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="40"/>
-      <c r="B73" s="81" t="s">
+      <c r="B73" s="98" t="s">
         <v>131</v>
       </c>
-      <c r="C73" s="81"/>
-      <c r="D73" s="81">
+      <c r="C73" s="98"/>
+      <c r="D73" s="98">
         <v>35.200000000000003</v>
       </c>
-      <c r="E73" s="81"/>
+      <c r="E73" s="98"/>
       <c r="F73" s="36" t="s">
         <v>15</v>
       </c>
@@ -8175,10 +8175,10 @@
       <c r="A74" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="B74" s="78" t="s">
+      <c r="B74" s="94" t="s">
         <v>133</v>
       </c>
-      <c r="C74" s="78"/>
+      <c r="C74" s="94"/>
       <c r="D74" s="45"/>
       <c r="E74" s="45"/>
       <c r="F74" s="36" t="s">
@@ -8258,10 +8258,10 @@
       <c r="A75" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="B75" s="78" t="s">
+      <c r="B75" s="94" t="s">
         <v>135</v>
       </c>
-      <c r="C75" s="78"/>
+      <c r="C75" s="94"/>
       <c r="D75" s="45"/>
       <c r="E75" s="45"/>
       <c r="F75" s="36" t="s">
@@ -8341,10 +8341,10 @@
       <c r="A76" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="B76" s="78" t="s">
+      <c r="B76" s="94" t="s">
         <v>137</v>
       </c>
-      <c r="C76" s="78"/>
+      <c r="C76" s="94"/>
       <c r="D76" s="45"/>
       <c r="E76" s="45"/>
       <c r="F76" s="36" t="s">
@@ -8425,10 +8425,10 @@
       <c r="A77" s="35">
         <v>0</v>
       </c>
-      <c r="B77" s="78" t="s">
+      <c r="B77" s="94" t="s">
         <v>138</v>
       </c>
-      <c r="C77" s="78"/>
+      <c r="C77" s="94"/>
       <c r="D77" s="45"/>
       <c r="E77" s="45"/>
       <c r="F77" s="36" t="s">
@@ -8508,10 +8508,10 @@
       <c r="A78" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="B78" s="78" t="s">
+      <c r="B78" s="94" t="s">
         <v>140</v>
       </c>
-      <c r="C78" s="78"/>
+      <c r="C78" s="94"/>
       <c r="D78" s="45"/>
       <c r="E78" s="45"/>
       <c r="F78" s="36" t="s">
@@ -8592,10 +8592,10 @@
       <c r="A79" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="B79" s="78" t="s">
+      <c r="B79" s="94" t="s">
         <v>142</v>
       </c>
-      <c r="C79" s="78"/>
+      <c r="C79" s="94"/>
       <c r="D79" s="45"/>
       <c r="E79" s="45"/>
       <c r="F79" s="36" t="s">
@@ -8676,10 +8676,10 @@
       <c r="A80" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="B80" s="78" t="s">
-        <v>252</v>
-      </c>
-      <c r="C80" s="78"/>
+      <c r="B80" s="94" t="s">
+        <v>254</v>
+      </c>
+      <c r="C80" s="94"/>
       <c r="D80" s="45"/>
       <c r="E80" s="45"/>
       <c r="F80" s="36" t="s">
@@ -8759,10 +8759,10 @@
       <c r="A81" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="B81" s="78" t="s">
+      <c r="B81" s="94" t="s">
         <v>145</v>
       </c>
-      <c r="C81" s="78"/>
+      <c r="C81" s="94"/>
       <c r="D81" s="45"/>
       <c r="E81" s="45"/>
       <c r="F81" s="36" t="s">
@@ -8842,10 +8842,10 @@
       <c r="A82" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="B82" s="78" t="s">
+      <c r="B82" s="94" t="s">
         <v>147</v>
       </c>
-      <c r="C82" s="78"/>
+      <c r="C82" s="94"/>
       <c r="D82" s="45"/>
       <c r="E82" s="45"/>
       <c r="F82" s="36" t="s">
@@ -8926,10 +8926,10 @@
       <c r="A83" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="B83" s="78" t="s">
+      <c r="B83" s="94" t="s">
         <v>149</v>
       </c>
-      <c r="C83" s="78"/>
+      <c r="C83" s="94"/>
       <c r="D83" s="45"/>
       <c r="E83" s="45"/>
       <c r="F83" s="36" t="s">
@@ -9010,10 +9010,10 @@
       <c r="A84" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="B84" s="78" t="s">
+      <c r="B84" s="94" t="s">
         <v>151</v>
       </c>
-      <c r="C84" s="78"/>
+      <c r="C84" s="94"/>
       <c r="D84" s="45"/>
       <c r="E84" s="45"/>
       <c r="F84" s="36" t="s">
@@ -9094,10 +9094,10 @@
       <c r="A85" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="B85" s="78" t="s">
+      <c r="B85" s="94" t="s">
         <v>153</v>
       </c>
-      <c r="C85" s="78"/>
+      <c r="C85" s="94"/>
       <c r="D85" s="45"/>
       <c r="E85" s="45"/>
       <c r="F85" s="36" t="s">
@@ -9178,10 +9178,10 @@
       <c r="A86" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="B86" s="78" t="s">
+      <c r="B86" s="94" t="s">
         <v>155</v>
       </c>
-      <c r="C86" s="78"/>
+      <c r="C86" s="94"/>
       <c r="D86" s="45"/>
       <c r="E86" s="45"/>
       <c r="F86" s="36" t="s">
@@ -9262,10 +9262,10 @@
       <c r="A87" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="B87" s="78" t="s">
+      <c r="B87" s="94" t="s">
         <v>157</v>
       </c>
-      <c r="C87" s="78"/>
+      <c r="C87" s="94"/>
       <c r="D87" s="45"/>
       <c r="E87" s="45"/>
       <c r="F87" s="36" t="s">
@@ -9346,10 +9346,10 @@
       <c r="A88" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="B88" s="78" t="s">
+      <c r="B88" s="94" t="s">
         <v>159</v>
       </c>
-      <c r="C88" s="78"/>
+      <c r="C88" s="94"/>
       <c r="D88" s="45"/>
       <c r="E88" s="45"/>
       <c r="F88" s="36" t="s">
@@ -9429,10 +9429,10 @@
       <c r="A89" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="B89" s="78" t="s">
+      <c r="B89" s="94" t="s">
         <v>161</v>
       </c>
-      <c r="C89" s="78"/>
+      <c r="C89" s="94"/>
       <c r="D89" s="45"/>
       <c r="E89" s="45"/>
       <c r="F89" s="36" t="s">
@@ -9512,10 +9512,10 @@
       <c r="A90" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="B90" s="78" t="s">
-        <v>253</v>
-      </c>
-      <c r="C90" s="78"/>
+      <c r="B90" s="94" t="s">
+        <v>252</v>
+      </c>
+      <c r="C90" s="94"/>
       <c r="D90" s="45"/>
       <c r="E90" s="45"/>
       <c r="F90" s="36" t="s">
@@ -9595,10 +9595,10 @@
       <c r="A91" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="B91" s="78" t="s">
+      <c r="B91" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C91" s="78"/>
+      <c r="C91" s="94"/>
       <c r="D91" s="45"/>
       <c r="E91" s="45"/>
       <c r="F91" s="36" t="s">
@@ -9678,10 +9678,10 @@
       <c r="A92" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="B92" s="78" t="s">
+      <c r="B92" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C92" s="78"/>
+      <c r="C92" s="94"/>
       <c r="D92" s="45"/>
       <c r="E92" s="45"/>
       <c r="F92" s="36" t="s">
@@ -9761,10 +9761,10 @@
       <c r="A93" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="B93" s="78" t="s">
+      <c r="B93" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C93" s="78"/>
+      <c r="C93" s="94"/>
       <c r="D93" s="45"/>
       <c r="E93" s="45"/>
       <c r="F93" s="36" t="s">
@@ -9844,10 +9844,10 @@
       <c r="A94" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="B94" s="78" t="s">
+      <c r="B94" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C94" s="78"/>
+      <c r="C94" s="94"/>
       <c r="D94" s="45"/>
       <c r="E94" s="45"/>
       <c r="F94" s="36" t="s">
@@ -9927,10 +9927,10 @@
       <c r="A95" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="B95" s="78" t="s">
+      <c r="B95" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C95" s="78"/>
+      <c r="C95" s="94"/>
       <c r="D95" s="45"/>
       <c r="E95" s="45"/>
       <c r="F95" s="36" t="s">
@@ -10010,10 +10010,10 @@
       <c r="A96" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="B96" s="78" t="s">
+      <c r="B96" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C96" s="78"/>
+      <c r="C96" s="94"/>
       <c r="D96" s="45"/>
       <c r="E96" s="45"/>
       <c r="F96" s="36" t="s">
@@ -10093,10 +10093,10 @@
       <c r="A97" s="35" t="s">
         <v>169</v>
       </c>
-      <c r="B97" s="78" t="s">
+      <c r="B97" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C97" s="78"/>
+      <c r="C97" s="94"/>
       <c r="D97" s="45"/>
       <c r="E97" s="45"/>
       <c r="F97" s="36" t="s">
@@ -10176,10 +10176,10 @@
       <c r="A98" s="35" t="s">
         <v>170</v>
       </c>
-      <c r="B98" s="78" t="s">
+      <c r="B98" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C98" s="78"/>
+      <c r="C98" s="94"/>
       <c r="D98" s="45"/>
       <c r="E98" s="45"/>
       <c r="F98" s="36" t="s">
@@ -10259,10 +10259,10 @@
       <c r="A99" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="B99" s="78" t="s">
+      <c r="B99" s="94" t="s">
         <v>172</v>
       </c>
-      <c r="C99" s="78"/>
+      <c r="C99" s="94"/>
       <c r="D99" s="45"/>
       <c r="E99" s="45"/>
       <c r="F99" s="36" t="s">
@@ -10342,10 +10342,10 @@
       <c r="A100" s="35" t="s">
         <v>173</v>
       </c>
-      <c r="B100" s="78" t="s">
+      <c r="B100" s="94" t="s">
         <v>174</v>
       </c>
-      <c r="C100" s="78"/>
+      <c r="C100" s="94"/>
       <c r="D100" s="45"/>
       <c r="E100" s="45"/>
       <c r="F100" s="36" t="s">
@@ -10425,10 +10425,10 @@
       <c r="A101" s="35" t="s">
         <v>175</v>
       </c>
-      <c r="B101" s="79" t="s">
+      <c r="B101" s="99" t="s">
         <v>176</v>
       </c>
-      <c r="C101" s="79"/>
+      <c r="C101" s="99"/>
       <c r="D101" s="45"/>
       <c r="E101" s="45"/>
       <c r="F101" s="36" t="s">
@@ -10508,10 +10508,10 @@
       <c r="A102" s="35" t="s">
         <v>177</v>
       </c>
-      <c r="B102" s="78" t="s">
+      <c r="B102" s="94" t="s">
         <v>178</v>
       </c>
-      <c r="C102" s="78"/>
+      <c r="C102" s="94"/>
       <c r="D102" s="45"/>
       <c r="E102" s="45"/>
       <c r="F102" s="36" t="s">
@@ -10591,10 +10591,10 @@
       <c r="A103" s="35" t="s">
         <v>179</v>
       </c>
-      <c r="B103" s="78" t="s">
+      <c r="B103" s="94" t="s">
         <v>180</v>
       </c>
-      <c r="C103" s="78"/>
+      <c r="C103" s="94"/>
       <c r="D103" s="45"/>
       <c r="E103" s="45"/>
       <c r="F103" s="36" t="s">
@@ -10674,10 +10674,10 @@
       <c r="A104" s="35" t="s">
         <v>181</v>
       </c>
-      <c r="B104" s="78" t="s">
+      <c r="B104" s="94" t="s">
         <v>182</v>
       </c>
-      <c r="C104" s="78"/>
+      <c r="C104" s="94"/>
       <c r="D104" s="45"/>
       <c r="E104" s="45"/>
       <c r="F104" s="36" t="s">
@@ -10757,10 +10757,10 @@
       <c r="A105" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="B105" s="78" t="s">
+      <c r="B105" s="94" t="s">
         <v>184</v>
       </c>
-      <c r="C105" s="78"/>
+      <c r="C105" s="94"/>
       <c r="D105" s="45"/>
       <c r="E105" s="45"/>
       <c r="F105" s="36" t="s">
@@ -10840,10 +10840,10 @@
       <c r="A106" s="35" t="s">
         <v>185</v>
       </c>
-      <c r="B106" s="78" t="s">
+      <c r="B106" s="94" t="s">
         <v>186</v>
       </c>
-      <c r="C106" s="78"/>
+      <c r="C106" s="94"/>
       <c r="D106" s="45"/>
       <c r="E106" s="45"/>
       <c r="F106" s="36" t="s">
@@ -10923,10 +10923,10 @@
       <c r="A107" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="B107" s="78" t="s">
+      <c r="B107" s="94" t="s">
         <v>188</v>
       </c>
-      <c r="C107" s="78"/>
+      <c r="C107" s="94"/>
       <c r="D107" s="45"/>
       <c r="E107" s="45"/>
       <c r="F107" s="36" t="s">
@@ -11006,10 +11006,10 @@
       <c r="A108" s="35" t="s">
         <v>189</v>
       </c>
-      <c r="B108" s="79" t="s">
+      <c r="B108" s="99" t="s">
         <v>190</v>
       </c>
-      <c r="C108" s="79"/>
+      <c r="C108" s="99"/>
       <c r="D108" s="45"/>
       <c r="E108" s="45"/>
       <c r="F108" s="36" t="s">
@@ -11089,10 +11089,10 @@
       <c r="A109" s="35" t="s">
         <v>191</v>
       </c>
-      <c r="B109" s="79" t="s">
+      <c r="B109" s="99" t="s">
         <v>190</v>
       </c>
-      <c r="C109" s="79"/>
+      <c r="C109" s="99"/>
       <c r="D109" s="45"/>
       <c r="E109" s="45"/>
       <c r="F109" s="36" t="s">
@@ -11172,10 +11172,10 @@
       <c r="A110" s="35" t="s">
         <v>192</v>
       </c>
-      <c r="B110" s="79" t="s">
+      <c r="B110" s="99" t="s">
         <v>190</v>
       </c>
-      <c r="C110" s="79"/>
+      <c r="C110" s="99"/>
       <c r="D110" s="45"/>
       <c r="E110" s="45"/>
       <c r="F110" s="36" t="s">
@@ -11255,10 +11255,10 @@
       <c r="A111" s="35" t="s">
         <v>193</v>
       </c>
-      <c r="B111" s="79" t="s">
+      <c r="B111" s="99" t="s">
         <v>190</v>
       </c>
-      <c r="C111" s="79"/>
+      <c r="C111" s="99"/>
       <c r="D111" s="45"/>
       <c r="E111" s="45"/>
       <c r="F111" s="36" t="s">
@@ -11338,10 +11338,10 @@
       <c r="A112" s="35" t="s">
         <v>194</v>
       </c>
-      <c r="B112" s="79" t="s">
+      <c r="B112" s="99" t="s">
         <v>190</v>
       </c>
-      <c r="C112" s="79"/>
+      <c r="C112" s="99"/>
       <c r="D112" s="45"/>
       <c r="E112" s="45"/>
       <c r="F112" s="36" t="s">
@@ -11421,10 +11421,10 @@
       <c r="A113" s="35" t="s">
         <v>195</v>
       </c>
-      <c r="B113" s="79" t="s">
+      <c r="B113" s="99" t="s">
         <v>190</v>
       </c>
-      <c r="C113" s="79"/>
+      <c r="C113" s="99"/>
       <c r="D113" s="45"/>
       <c r="E113" s="45"/>
       <c r="F113" s="36" t="s">
@@ -11504,10 +11504,10 @@
       <c r="A114" s="35" t="s">
         <v>196</v>
       </c>
-      <c r="B114" s="79" t="s">
+      <c r="B114" s="99" t="s">
         <v>190</v>
       </c>
-      <c r="C114" s="79"/>
+      <c r="C114" s="99"/>
       <c r="D114" s="45"/>
       <c r="E114" s="45"/>
       <c r="F114" s="36" t="s">
@@ -11587,10 +11587,10 @@
       <c r="A115" s="35" t="s">
         <v>197</v>
       </c>
-      <c r="B115" s="78" t="s">
+      <c r="B115" s="94" t="s">
         <v>198</v>
       </c>
-      <c r="C115" s="78"/>
+      <c r="C115" s="94"/>
       <c r="D115" s="45"/>
       <c r="E115" s="45"/>
       <c r="F115" s="36" t="s">
@@ -11670,10 +11670,10 @@
       <c r="A116" s="35" t="s">
         <v>199</v>
       </c>
-      <c r="B116" s="78" t="s">
+      <c r="B116" s="94" t="s">
         <v>200</v>
       </c>
-      <c r="C116" s="78"/>
+      <c r="C116" s="94"/>
       <c r="D116" s="45"/>
       <c r="E116" s="45"/>
       <c r="F116" s="36" t="s">
@@ -11753,10 +11753,10 @@
       <c r="A117" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="B117" s="78" t="s">
+      <c r="B117" s="94" t="s">
         <v>202</v>
       </c>
-      <c r="C117" s="78"/>
+      <c r="C117" s="94"/>
       <c r="D117" s="45"/>
       <c r="E117" s="45"/>
       <c r="F117" s="36" t="s">
@@ -11836,10 +11836,10 @@
       <c r="A118" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="B118" s="78" t="s">
+      <c r="B118" s="94" t="s">
         <v>204</v>
       </c>
-      <c r="C118" s="78"/>
+      <c r="C118" s="94"/>
       <c r="D118" s="45"/>
       <c r="E118" s="45"/>
       <c r="F118" s="36" t="s">
@@ -11919,10 +11919,10 @@
       <c r="A119" s="35" t="s">
         <v>205</v>
       </c>
-      <c r="B119" s="78" t="s">
+      <c r="B119" s="94" t="s">
         <v>206</v>
       </c>
-      <c r="C119" s="78"/>
+      <c r="C119" s="94"/>
       <c r="D119" s="45"/>
       <c r="E119" s="45"/>
       <c r="F119" s="36" t="s">
@@ -12003,10 +12003,10 @@
       <c r="A120" s="35" t="s">
         <v>207</v>
       </c>
-      <c r="B120" s="78" t="s">
+      <c r="B120" s="94" t="s">
         <v>208</v>
       </c>
-      <c r="C120" s="78"/>
+      <c r="C120" s="94"/>
       <c r="D120" s="45"/>
       <c r="E120" s="45"/>
       <c r="F120" s="36" t="s">
@@ -12087,10 +12087,10 @@
       <c r="A121" s="35" t="s">
         <v>209</v>
       </c>
-      <c r="B121" s="78" t="s">
+      <c r="B121" s="94" t="s">
         <v>210</v>
       </c>
-      <c r="C121" s="78"/>
+      <c r="C121" s="94"/>
       <c r="D121" s="45"/>
       <c r="E121" s="45"/>
       <c r="F121" s="36" t="s">
@@ -12170,10 +12170,10 @@
       <c r="A122" s="35" t="s">
         <v>211</v>
       </c>
-      <c r="B122" s="78" t="s">
+      <c r="B122" s="94" t="s">
         <v>212</v>
       </c>
-      <c r="C122" s="78"/>
+      <c r="C122" s="94"/>
       <c r="D122" s="45"/>
       <c r="E122" s="45"/>
       <c r="F122" s="36" t="s">
@@ -12253,10 +12253,10 @@
       <c r="A123" s="35" t="s">
         <v>213</v>
       </c>
-      <c r="B123" s="78" t="s">
+      <c r="B123" s="94" t="s">
         <v>214</v>
       </c>
-      <c r="C123" s="78"/>
+      <c r="C123" s="94"/>
       <c r="D123" s="45"/>
       <c r="E123" s="45"/>
       <c r="F123" s="36" t="s">
@@ -12336,10 +12336,10 @@
       <c r="A124" s="35" t="s">
         <v>215</v>
       </c>
-      <c r="B124" s="78" t="s">
+      <c r="B124" s="94" t="s">
         <v>216</v>
       </c>
-      <c r="C124" s="78"/>
+      <c r="C124" s="94"/>
       <c r="D124" s="45"/>
       <c r="E124" s="45"/>
       <c r="F124" s="36" t="s">
@@ -12419,10 +12419,10 @@
       <c r="A125" s="35" t="s">
         <v>217</v>
       </c>
-      <c r="B125" s="78" t="s">
+      <c r="B125" s="94" t="s">
         <v>218</v>
       </c>
-      <c r="C125" s="78"/>
+      <c r="C125" s="94"/>
       <c r="D125" s="45"/>
       <c r="E125" s="45"/>
       <c r="F125" s="36" t="s">
@@ -12502,10 +12502,10 @@
       <c r="A126" s="35" t="s">
         <v>219</v>
       </c>
-      <c r="B126" s="78" t="s">
+      <c r="B126" s="94" t="s">
         <v>220</v>
       </c>
-      <c r="C126" s="78"/>
+      <c r="C126" s="94"/>
       <c r="D126" s="45"/>
       <c r="E126" s="45"/>
       <c r="F126" s="36" t="s">
@@ -12585,10 +12585,10 @@
       <c r="A127" s="35" t="s">
         <v>221</v>
       </c>
-      <c r="B127" s="78" t="s">
+      <c r="B127" s="94" t="s">
         <v>222</v>
       </c>
-      <c r="C127" s="78"/>
+      <c r="C127" s="94"/>
       <c r="D127" s="45"/>
       <c r="E127" s="45"/>
       <c r="F127" s="36" t="s">
@@ -12668,10 +12668,10 @@
       <c r="A128" s="35" t="s">
         <v>223</v>
       </c>
-      <c r="B128" s="78" t="s">
+      <c r="B128" s="94" t="s">
         <v>224</v>
       </c>
-      <c r="C128" s="78"/>
+      <c r="C128" s="94"/>
       <c r="D128" s="45"/>
       <c r="E128" s="45"/>
       <c r="F128" s="36" t="s">
@@ -12751,10 +12751,10 @@
       <c r="A129" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="B129" s="78" t="s">
+      <c r="B129" s="94" t="s">
         <v>226</v>
       </c>
-      <c r="C129" s="78"/>
+      <c r="C129" s="94"/>
       <c r="D129" s="45"/>
       <c r="E129" s="45"/>
       <c r="F129" s="36" t="s">
@@ -12834,10 +12834,10 @@
       <c r="A130" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="B130" s="78" t="s">
+      <c r="B130" s="94" t="s">
         <v>228</v>
       </c>
-      <c r="C130" s="78"/>
+      <c r="C130" s="94"/>
       <c r="D130" s="45"/>
       <c r="E130" s="45"/>
       <c r="F130" s="36" t="s">
@@ -12917,10 +12917,10 @@
       <c r="A131" s="35" t="s">
         <v>229</v>
       </c>
-      <c r="B131" s="77" t="s">
+      <c r="B131" s="91" t="s">
         <v>230</v>
       </c>
-      <c r="C131" s="77"/>
+      <c r="C131" s="91"/>
       <c r="D131" s="36"/>
       <c r="E131" s="36"/>
       <c r="F131" s="36" t="s">
@@ -13231,7 +13231,7 @@
       <c r="D132" s="55"/>
       <c r="E132" s="49"/>
       <c r="F132" s="56" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G132" s="49"/>
       <c r="H132" s="57"/>
@@ -14186,6 +14186,133 @@
     </row>
   </sheetData>
   <mergeCells count="141">
+    <mergeCell ref="B131:C131"/>
+    <mergeCell ref="B122:C122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B126:C126"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="B129:C129"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="B118:C118"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="B121:C121"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B97:C97"/>
+    <mergeCell ref="B98:C98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B90:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B94:C94"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B82:C82"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B67:C67"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="A2:U2"/>
     <mergeCell ref="J5:K5"/>
@@ -14200,133 +14327,6 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:S7"/>
     <mergeCell ref="T7:U7"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B97:C97"/>
-    <mergeCell ref="B98:C98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B114:C114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="B118:C118"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="B121:C121"/>
-    <mergeCell ref="B131:C131"/>
-    <mergeCell ref="B122:C122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B126:C126"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="B129:C129"/>
-    <mergeCell ref="B130:C130"/>
   </mergeCells>
   <phoneticPr fontId="26" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>